<commit_message>
Added total fleet numbers and fixed multi
</commit_message>
<xml_diff>
--- a/results/Manuscript/material_use.xlsx
+++ b/results/Manuscript/material_use.xlsx
@@ -117,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="111">
+  <fills count="110">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,12 +468,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE4FEE4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF028102"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -540,7 +534,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2E992E"/>
+        <fgColor rgb="FF2D992D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,6 +618,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF55AF55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF54AE54"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -684,7 +684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6A6A"/>
+        <fgColor rgb="FFFF6B6B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,12 +739,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBEBE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6B6B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -869,14 +863,14 @@
     <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -920,7 +914,6 @@
     <xf numFmtId="0" fontId="2" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="109" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="110" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="3">
-        <v>38466.83838074606</v>
+        <v>38465.27478711109</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1275,7 +1268,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="4">
-        <v>39016.02447409456</v>
+        <v>39014.46088045958</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1295,7 +1288,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5">
-        <v>39569.18819264948</v>
+        <v>39567.62459901452</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1315,7 +1308,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="6">
-        <v>40245.38816861642</v>
+        <v>40243.82457498145</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1335,7 +1328,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="7">
-        <v>37730.99709115538</v>
+        <v>37730.95593699767</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1355,7 +1348,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="7">
-        <v>37762.77907556015</v>
+        <v>37762.73792140245</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1375,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="8">
-        <v>37799.93149266503</v>
+        <v>37799.89033850733</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1395,7 +1388,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="7">
-        <v>37770.90343925087</v>
+        <v>37770.86228509317</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1415,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="7">
-        <v>37684.81901846525</v>
+        <v>37684.73314062999</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1435,7 +1428,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="7">
-        <v>37696.8463231445</v>
+        <v>37696.76044530924</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1455,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="7">
-        <v>37711.53386597138</v>
+        <v>37711.44798813612</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1475,7 +1468,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="7">
-        <v>37707.46379757278</v>
+        <v>37707.37791973752</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1495,7 +1488,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="7">
-        <v>37669.8426234517</v>
+        <v>37669.82332127394</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1515,7 +1508,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="7">
-        <v>37672.42634054396</v>
+        <v>37672.37795973063</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1535,7 +1528,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="7">
-        <v>37676.26279065417</v>
+        <v>37676.14093637807</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1555,7 +1548,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="7">
-        <v>37679.1264945474</v>
+        <v>37679.07811373407</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1635,7 +1628,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="7">
-        <v>37667.47153277695</v>
+        <v>37667.35120952562</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1735,7 +1728,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="9">
-        <v>38220.86882253804</v>
+        <v>38220.06094604808</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1755,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="10">
-        <v>38618.24672364227</v>
+        <v>38617.42402687058</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1775,7 +1768,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="4">
-        <v>39021.39408143059</v>
+        <v>39020.55188893808</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1795,7 +1788,7 @@
         <v>17</v>
       </c>
       <c r="F29" s="5">
-        <v>39559.1764287118</v>
+        <v>39558.28047158827</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1815,7 +1808,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="11">
-        <v>38507.5126016381</v>
+        <v>38507.471510018</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1835,7 +1828,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="12">
-        <v>38536.49624959972</v>
+        <v>38536.45516180197</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1855,7 +1848,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="12">
-        <v>38572.01405788543</v>
+        <v>38571.97291141397</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1875,7 +1868,7 @@
         <v>17</v>
       </c>
       <c r="F33" s="12">
-        <v>38543.36395181112</v>
+        <v>38543.32280533967</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1895,7 +1888,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="11">
-        <v>38497.47784302043</v>
+        <v>38497.4501283091</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1915,7 +1908,7 @@
         <v>16</v>
       </c>
       <c r="F35" s="11">
-        <v>38501.65332961389</v>
+        <v>38501.62561490256</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1935,7 +1928,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="11">
-        <v>38506.76411821543</v>
+        <v>38506.7364035041</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1955,7 +1948,7 @@
         <v>17</v>
       </c>
       <c r="F37" s="11">
-        <v>38506.18888679553</v>
+        <v>38506.1611720842</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1975,7 +1968,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="11">
-        <v>38504.01082036334</v>
+        <v>38503.9950241257</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1995,7 +1988,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="11">
-        <v>38504.94258463182</v>
+        <v>38504.92678839416</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2015,7 +2008,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="11">
-        <v>38502.69291321689</v>
+        <v>38502.65309035227</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2035,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="F41" s="11">
-        <v>38503.99116043323</v>
+        <v>38503.95133756861</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2115,7 +2108,7 @@
         <v>17</v>
       </c>
       <c r="F45" s="11">
-        <v>38510.45582504639</v>
+        <v>38513.92842738284</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2215,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="13">
-        <v>38748.72302609441</v>
+        <v>38747.1458241467</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2235,7 +2228,7 @@
         <v>16</v>
       </c>
       <c r="F51" s="14">
-        <v>39344.37066689577</v>
+        <v>39342.87160938028</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2255,7 +2248,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="15">
-        <v>39889.51858655626</v>
+        <v>39888.04134533925</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2275,7 +2268,7 @@
         <v>17</v>
       </c>
       <c r="F53" s="16">
-        <v>40638.2274232596</v>
+        <v>40636.79097634733</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2295,7 +2288,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="17">
-        <v>44466.85107263732</v>
+        <v>44466.82391280789</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2315,7 +2308,7 @@
         <v>16</v>
       </c>
       <c r="F55" s="18">
-        <v>44490.74514540662</v>
+        <v>44490.7179855772</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2335,7 +2328,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="18">
-        <v>44518.87612696919</v>
+        <v>44518.84896713976</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2355,7 +2348,7 @@
         <v>17</v>
       </c>
       <c r="F57" s="18">
-        <v>44501.42453776985</v>
+        <v>44501.39737794043</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2375,7 +2368,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="18">
-        <v>44502.602783503</v>
+        <v>44502.54340055366</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2395,7 +2388,7 @@
         <v>16</v>
       </c>
       <c r="F59" s="18">
-        <v>44511.84304376446</v>
+        <v>44511.78366081511</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2415,7 +2408,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="18">
-        <v>44523.16188609542</v>
+        <v>44523.10250314605</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2435,7 +2428,7 @@
         <v>17</v>
       </c>
       <c r="F61" s="18">
-        <v>44522.2121149448</v>
+        <v>44522.15273199545</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2455,7 +2448,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="19">
-        <v>44589.90419191646</v>
+        <v>44589.8691446212</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2475,7 +2468,7 @@
         <v>16</v>
       </c>
       <c r="F63" s="20">
-        <v>44592.00731591836</v>
+        <v>44591.9722686231</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2495,7 +2488,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="19">
-        <v>44562.9288488478</v>
+        <v>44562.84107027439</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2515,7 +2508,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="19">
-        <v>44565.970637422</v>
+        <v>44565.88285884861</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2595,7 +2588,7 @@
         <v>17</v>
       </c>
       <c r="F69" s="22">
-        <v>44657.14791980329</v>
+        <v>44688.82472181291</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2695,7 +2688,7 @@
         <v>11</v>
       </c>
       <c r="F74" s="23">
-        <v>41207.60473052369</v>
+        <v>41205.88741284297</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2715,7 +2708,7 @@
         <v>16</v>
       </c>
       <c r="F75" s="24">
-        <v>41756.79082387219</v>
+        <v>41755.07350619146</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2735,7 +2728,7 @@
         <v>13</v>
       </c>
       <c r="F76" s="25">
-        <v>42309.95454242711</v>
+        <v>42308.23722474639</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2755,7 +2748,7 @@
         <v>17</v>
       </c>
       <c r="F77" s="26">
-        <v>42986.15451839405</v>
+        <v>42984.43720071333</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2775,7 +2768,7 @@
         <v>11</v>
       </c>
       <c r="F78" s="27">
-        <v>40454.90781617587</v>
+        <v>40454.88963445497</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2795,7 +2788,7 @@
         <v>16</v>
       </c>
       <c r="F79" s="28">
-        <v>40474.56082464437</v>
+        <v>40474.54264292348</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2815,7 +2808,7 @@
         <v>13</v>
       </c>
       <c r="F80" s="28">
-        <v>40505.60995645622</v>
+        <v>40505.48172590999</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2835,7 +2828,7 @@
         <v>17</v>
       </c>
       <c r="F81" s="28">
-        <v>40484.75477039215</v>
+        <v>40484.73658867125</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2855,7 +2848,7 @@
         <v>11</v>
       </c>
       <c r="F82" s="27">
-        <v>40418.88316793256</v>
+        <v>40418.86709466899</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2875,7 +2868,7 @@
         <v>16</v>
       </c>
       <c r="F83" s="27">
-        <v>40424.23798751682</v>
+        <v>40424.17426154265</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2895,7 +2888,7 @@
         <v>13</v>
       </c>
       <c r="F84" s="27">
-        <v>40433.29975206833</v>
+        <v>40433.23602609416</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2915,7 +2908,7 @@
         <v>17</v>
       </c>
       <c r="F85" s="27">
-        <v>40434.02525596179</v>
+        <v>40433.96152998762</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2935,7 +2928,7 @@
         <v>11</v>
       </c>
       <c r="F86" s="27">
-        <v>40410.6788216164</v>
+        <v>40410.66945720912</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2955,7 +2948,7 @@
         <v>16</v>
       </c>
       <c r="F87" s="27">
-        <v>40411.67375059154</v>
+        <v>40411.66438618426</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2975,7 +2968,7 @@
         <v>13</v>
       </c>
       <c r="F88" s="27">
-        <v>40413.4054796498</v>
+        <v>40413.37642507819</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2995,7 +2988,7 @@
         <v>17</v>
       </c>
       <c r="F89" s="27">
-        <v>40416.52922482019</v>
+        <v>40416.50017024858</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3175,7 +3168,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="29">
-        <v>40939.8918483761</v>
+        <v>40938.89661601398</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3195,7 +3188,7 @@
         <v>16</v>
       </c>
       <c r="F99" s="30">
-        <v>41321.02545101201</v>
+        <v>41320.02067447848</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3215,7 +3208,7 @@
         <v>13</v>
       </c>
       <c r="F100" s="31">
-        <v>41713.44765744992</v>
+        <v>41712.42424762417</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3235,7 +3228,7 @@
         <v>17</v>
       </c>
       <c r="F101" s="32">
-        <v>42180.11791177165</v>
+        <v>42179.02396933924</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3255,7 +3248,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="24">
-        <v>41757.35005607025</v>
+        <v>41757.3318743456</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3275,7 +3268,7 @@
         <v>16</v>
       </c>
       <c r="F103" s="24">
-        <v>41777.00493369412</v>
+        <v>41776.98675197322</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3295,7 +3288,7 @@
         <v>13</v>
       </c>
       <c r="F104" s="33">
-        <v>41800.39402206728</v>
+        <v>41800.34093382565</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3315,7 +3308,7 @@
         <v>17</v>
       </c>
       <c r="F105" s="24">
-        <v>41787.19887944189</v>
+        <v>41787.180697721</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3335,7 +3328,7 @@
         <v>11</v>
       </c>
       <c r="F106" s="31">
-        <v>41736.3140430138</v>
+        <v>41736.31004208286</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3355,7 +3348,7 @@
         <v>16</v>
       </c>
       <c r="F107" s="31">
-        <v>41739.91550631755</v>
+        <v>41739.88405484702</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3375,7 +3368,7 @@
         <v>13</v>
       </c>
       <c r="F108" s="24">
-        <v>41747.10014731561</v>
+        <v>41747.03642134144</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3395,7 +3388,7 @@
         <v>17</v>
       </c>
       <c r="F109" s="24">
-        <v>41748.71140733389</v>
+        <v>41748.67995586335</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3415,7 +3408,7 @@
         <v>11</v>
       </c>
       <c r="F110" s="31">
-        <v>41734.43517062966</v>
+        <v>41734.43213710619</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3435,7 +3428,7 @@
         <v>16</v>
       </c>
       <c r="F111" s="31">
-        <v>41734.91175129175</v>
+        <v>41734.90676953557</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3455,7 +3448,7 @@
         <v>13</v>
       </c>
       <c r="F112" s="31">
-        <v>41735.72007032299</v>
+        <v>41735.70432949973</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3475,7 +3468,7 @@
         <v>17</v>
       </c>
       <c r="F113" s="31">
-        <v>41738.52407213709</v>
+        <v>41738.50833131382</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3655,7 +3648,7 @@
         <v>11</v>
       </c>
       <c r="F122" s="34">
-        <v>41453.43786320782</v>
+        <v>41451.4717268387</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3675,7 +3668,7 @@
         <v>16</v>
       </c>
       <c r="F123" s="35">
-        <v>42133.9611402068</v>
+        <v>42132.10293156586</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3695,7 +3688,7 @@
         <v>13</v>
       </c>
       <c r="F124" s="36">
-        <v>42742.5208180529</v>
+        <v>42740.70150034979</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3715,7 +3708,7 @@
         <v>17</v>
       </c>
       <c r="F125" s="37">
-        <v>43649.28565168451</v>
+        <v>43647.49738586253</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3735,7 +3728,7 @@
         <v>11</v>
       </c>
       <c r="F126" s="38">
-        <v>51378.11655002379</v>
+        <v>51378.10459256962</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3755,7 +3748,7 @@
         <v>16</v>
       </c>
       <c r="F127" s="38">
-        <v>51392.73233370257</v>
+        <v>51392.7203762484</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3775,7 +3768,7 @@
         <v>13</v>
       </c>
       <c r="F128" s="38">
-        <v>51397.89590622543</v>
+        <v>51397.80712297671</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3795,7 +3788,7 @@
         <v>17</v>
       </c>
       <c r="F129" s="38">
-        <v>51403.02130923652</v>
+        <v>51403.00941325721</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3815,7 +3808,7 @@
         <v>11</v>
       </c>
       <c r="F130" s="38">
-        <v>51392.46180800905</v>
+        <v>51392.45077803753</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3835,7 +3828,7 @@
         <v>16</v>
       </c>
       <c r="F131" s="38">
-        <v>51387.51428061179</v>
+        <v>51387.47096802077</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3855,7 +3848,7 @@
         <v>13</v>
       </c>
       <c r="F132" s="38">
-        <v>51394.38081371925</v>
+        <v>51394.33750112823</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3875,7 +3868,7 @@
         <v>17</v>
       </c>
       <c r="F133" s="38">
-        <v>51396.01372867237</v>
+        <v>51395.97041608134</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3895,7 +3888,7 @@
         <v>11</v>
       </c>
       <c r="F134" s="38">
-        <v>51401.79833223075</v>
+        <v>51401.79168828301</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3915,7 +3908,7 @@
         <v>16</v>
       </c>
       <c r="F135" s="38">
-        <v>51402.55276678043</v>
+        <v>51402.54612283271</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3935,7 +3928,7 @@
         <v>13</v>
       </c>
       <c r="F136" s="38">
-        <v>51400.40791876754</v>
+        <v>51400.38741980675</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3955,7 +3948,7 @@
         <v>17</v>
       </c>
       <c r="F137" s="38">
-        <v>51403.03628714607</v>
+        <v>51403.0157881853</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4165,7 +4158,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="39">
-        <v>7762.230904495669</v>
+        <v>7762.187402309328</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4185,7 +4178,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="40">
-        <v>7819.026426655899</v>
+        <v>7818.982924469557</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4205,7 +4198,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="41">
-        <v>7877.095302921653</v>
+        <v>7877.051800735312</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4225,7 +4218,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="42">
-        <v>7890.46350550753</v>
+        <v>7890.420003321188</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4245,7 +4238,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="43">
-        <v>7690.104977588864</v>
+        <v>7690.092865592277</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4265,7 +4258,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="43">
-        <v>7699.754227312374</v>
+        <v>7699.742115315785</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4285,7 +4278,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="44">
-        <v>7711.048389499818</v>
+        <v>7711.036277503229</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4305,7 +4298,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="43">
-        <v>7702.397696305205</v>
+        <v>7702.385584308618</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4325,7 +4318,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="43">
-        <v>7676.086457795165</v>
+        <v>7676.059647992612</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4345,7 +4338,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="43">
-        <v>7679.872141479203</v>
+        <v>7679.845331676649</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4365,7 +4358,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="43">
-        <v>7684.496152035683</v>
+        <v>7684.469342233129</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4385,7 +4378,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="43">
-        <v>7683.249722280518</v>
+        <v>7683.222912477964</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4405,7 +4398,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="43">
-        <v>7671.339218616151</v>
+        <v>7671.333045060452</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4425,7 +4418,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="43">
-        <v>7672.164983781145</v>
+        <v>7672.149534262048</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4445,7 +4438,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="43">
-        <v>7673.390166516975</v>
+        <v>7673.351379314943</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -4465,7 +4458,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="43">
-        <v>7674.307743067507</v>
+        <v>7674.29229354841</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4545,7 +4538,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="43">
-        <v>7670.580224704273</v>
+        <v>7670.541781585972</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4645,7 +4638,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="45">
-        <v>7432.871061972496</v>
+        <v>7433.461940002579</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -4665,7 +4658,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="46">
-        <v>7373.407983701895</v>
+        <v>7373.961576532868</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4685,7 +4678,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="47">
-        <v>7322.24910120504</v>
+        <v>7322.759082200902</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4705,7 +4698,7 @@
         <v>17</v>
       </c>
       <c r="F29" s="48">
-        <v>7220.412694556306</v>
+        <v>7220.820891655325</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4725,7 +4718,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="49">
-        <v>6836.262751965781</v>
+        <v>6836.250717622642</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4745,7 +4738,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="50">
-        <v>6841.634718008491</v>
+        <v>6841.622679708142</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4765,7 +4758,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="50">
-        <v>6849.579730426767</v>
+        <v>6849.567629135519</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4785,7 +4778,7 @@
         <v>17</v>
       </c>
       <c r="F33" s="50">
-        <v>6839.309432854832</v>
+        <v>6839.297331563585</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4805,7 +4798,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="50">
-        <v>6839.953517881658</v>
+        <v>6839.98123259299</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4825,7 +4818,7 @@
         <v>16</v>
       </c>
       <c r="F35" s="49">
-        <v>6835.778031288206</v>
+        <v>6835.805745999537</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4845,7 +4838,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="49">
-        <v>6830.667242686658</v>
+        <v>6830.694957397989</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4865,7 +4858,7 @@
         <v>17</v>
       </c>
       <c r="F37" s="49">
-        <v>6831.242474106565</v>
+        <v>6831.270188817896</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4885,7 +4878,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="49">
-        <v>6833.420540538747</v>
+        <v>6833.436336776395</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4905,7 +4898,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="49">
-        <v>6832.488776270274</v>
+        <v>6832.504572507923</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4925,7 +4918,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="49">
-        <v>6834.738447685204</v>
+        <v>6834.778270549823</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4945,7 +4938,7 @@
         <v>17</v>
       </c>
       <c r="F41" s="49">
-        <v>6833.440200468862</v>
+        <v>6833.480023333482</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -5025,7 +5018,7 @@
         <v>17</v>
       </c>
       <c r="F45" s="49">
-        <v>6826.975535855702</v>
+        <v>6823.502933519252</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -5125,7 +5118,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="51">
-        <v>6588.708334807691</v>
+        <v>6590.285536755401</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5145,7 +5138,7 @@
         <v>16</v>
       </c>
       <c r="F51" s="52">
-        <v>6187.904378293919</v>
+        <v>6189.270993553476</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -5165,7 +5158,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="53">
-        <v>5937.011243209198</v>
+        <v>5938.315755350531</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5185,7 +5178,7 @@
         <v>17</v>
       </c>
       <c r="F53" s="54">
-        <v>5361.725203361011</v>
+        <v>5362.894857524309</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -5205,7 +5198,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="55">
-        <v>870.5802882647909</v>
+        <v>870.6074480942096</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5225,7 +5218,7 @@
         <v>16</v>
       </c>
       <c r="F55" s="56">
-        <v>846.6862154954856</v>
+        <v>846.7133753249044</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5245,7 +5238,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="56">
-        <v>818.5552339329178</v>
+        <v>818.582393762337</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5265,7 +5258,7 @@
         <v>17</v>
       </c>
       <c r="F57" s="56">
-        <v>836.0068231322499</v>
+        <v>836.0339829616685</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5285,7 +5278,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="56">
-        <v>834.828577399082</v>
+        <v>834.8879603484418</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5305,7 +5298,7 @@
         <v>16</v>
       </c>
       <c r="F59" s="56">
-        <v>825.5883171376208</v>
+        <v>825.6477000869809</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5325,7 +5318,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="56">
-        <v>814.269474806686</v>
+        <v>814.3288577560461</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -5345,7 +5338,7 @@
         <v>17</v>
       </c>
       <c r="F61" s="56">
-        <v>815.2192459572987</v>
+        <v>815.2786289066586</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -5365,7 +5358,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="57">
-        <v>747.5271689856309</v>
+        <v>747.562216280891</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -5385,7 +5378,7 @@
         <v>16</v>
       </c>
       <c r="F63" s="57">
-        <v>745.4240449837337</v>
+        <v>745.4590922789937</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -5405,7 +5398,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="58">
-        <v>774.5025120542956</v>
+        <v>774.5902906276995</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5425,7 +5418,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="58">
-        <v>771.4607234800824</v>
+        <v>771.5485020534869</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5504,8 +5497,8 @@
       <c r="E69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F69" s="60">
-        <v>680.2834410988144</v>
+      <c r="F69" s="59">
+        <v>648.6066390891856</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5604,8 +5597,8 @@
       <c r="E74" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F74" s="61">
-        <v>12148.77695620095</v>
+      <c r="F74" s="60">
+        <v>12148.68467526158</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -5624,8 +5617,8 @@
       <c r="E75" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F75" s="62">
-        <v>12205.57247836118</v>
+      <c r="F75" s="61">
+        <v>12205.48019742181</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -5644,8 +5637,8 @@
       <c r="E76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="63">
-        <v>12263.64135462694</v>
+      <c r="F76" s="62">
+        <v>12263.54907368757</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -5664,8 +5657,8 @@
       <c r="E77" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F77" s="63">
-        <v>12277.00955721282</v>
+      <c r="F77" s="62">
+        <v>12276.91727627344</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -5684,8 +5677,8 @@
       <c r="E78" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="64">
-        <v>12072.01404723274</v>
+      <c r="F78" s="63">
+        <v>12072.00850882874</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -5704,8 +5697,8 @@
       <c r="E79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="64">
-        <v>12078.11437111027</v>
+      <c r="F79" s="63">
+        <v>12078.10883270627</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -5724,8 +5717,8 @@
       <c r="E80" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="64">
-        <v>12087.62271831749</v>
+      <c r="F80" s="63">
+        <v>12087.58497974073</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -5744,8 +5737,8 @@
       <c r="E81" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F81" s="64">
-        <v>12081.36339767789</v>
+      <c r="F81" s="63">
+        <v>12081.3578592739</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -5764,8 +5757,8 @@
       <c r="E82" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F82" s="64">
-        <v>12060.84963450486</v>
+      <c r="F82" s="63">
+        <v>12060.84452287378</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -5784,8 +5777,8 @@
       <c r="E83" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="64">
-        <v>12062.55347390027</v>
+      <c r="F83" s="63">
+        <v>12062.53334661619</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -5804,8 +5797,8 @@
       <c r="E84" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F84" s="64">
-        <v>12065.4295273276</v>
+      <c r="F84" s="63">
+        <v>12065.40940004352</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -5824,8 +5817,8 @@
       <c r="E85" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F85" s="64">
-        <v>12065.67310559727</v>
+      <c r="F85" s="63">
+        <v>12065.65297831319</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -5844,8 +5837,8 @@
       <c r="E86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F86" s="64">
-        <v>12058.23314021843</v>
+      <c r="F86" s="63">
+        <v>12058.23014303757</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -5864,8 +5857,8 @@
       <c r="E87" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="64">
-        <v>12058.55164473398</v>
+      <c r="F87" s="63">
+        <v>12058.54864755312</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -5884,8 +5877,8 @@
       <c r="E88" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F88" s="64">
-        <v>12059.10580824002</v>
+      <c r="F88" s="63">
+        <v>12059.09651642851</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -5904,8 +5897,8 @@
       <c r="E89" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="64">
-        <v>12060.10572977944</v>
+      <c r="F89" s="63">
+        <v>12060.09643796792</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -5924,7 +5917,7 @@
       <c r="E90" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F90" s="64">
+      <c r="F90" s="63">
         <v>12057.72662512459</v>
       </c>
     </row>
@@ -5944,7 +5937,7 @@
       <c r="E91" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="64">
+      <c r="F91" s="63">
         <v>12057.72662512459</v>
       </c>
     </row>
@@ -5964,7 +5957,7 @@
       <c r="E92" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F92" s="64">
+      <c r="F92" s="63">
         <v>12057.72662512459</v>
       </c>
     </row>
@@ -5984,7 +5977,7 @@
       <c r="E93" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F93" s="64">
+      <c r="F93" s="63">
         <v>12057.88115032625</v>
       </c>
     </row>
@@ -6004,7 +5997,7 @@
       <c r="E94" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F94" s="64">
+      <c r="F94" s="63">
         <v>12057.75609937997</v>
       </c>
     </row>
@@ -6024,7 +6017,7 @@
       <c r="E95" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="64">
+      <c r="F95" s="63">
         <v>12057.79923312575</v>
       </c>
     </row>
@@ -6044,7 +6037,7 @@
       <c r="E96" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F96" s="64">
+      <c r="F96" s="63">
         <v>12057.85381130493</v>
       </c>
     </row>
@@ -6064,7 +6057,7 @@
       <c r="E97" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F97" s="64">
+      <c r="F97" s="63">
         <v>12058.1392081003</v>
       </c>
     </row>
@@ -6084,8 +6077,8 @@
       <c r="E98" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="65">
-        <v>11751.69923264933</v>
+      <c r="F98" s="64">
+        <v>11752.39785298662</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -6104,8 +6097,8 @@
       <c r="E99" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="66">
-        <v>11639.50065960059</v>
+      <c r="F99" s="65">
+        <v>11640.1433753834</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -6124,8 +6117,8 @@
       <c r="E100" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F100" s="67">
-        <v>11558.58473979691</v>
+      <c r="F100" s="66">
+        <v>11559.17384620724</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -6144,8 +6137,8 @@
       <c r="E101" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F101" s="68">
-        <v>11307.86417669644</v>
+      <c r="F101" s="67">
+        <v>11308.27319372128</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -6164,8 +6157,8 @@
       <c r="E102" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F102" s="69">
-        <v>10739.36864785224</v>
+      <c r="F102" s="68">
+        <v>10739.36310945461</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -6184,8 +6177,8 @@
       <c r="E103" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F103" s="69">
-        <v>10745.46558138765</v>
+      <c r="F103" s="68">
+        <v>10745.46004298365</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -6204,8 +6197,8 @@
       <c r="E104" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="69">
-        <v>10752.94826330661</v>
+      <c r="F104" s="68">
+        <v>10752.97763142335</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -6224,8 +6217,8 @@
       <c r="E105" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F105" s="69">
-        <v>10748.71460795527</v>
+      <c r="F105" s="68">
+        <v>10748.70906955127</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -6244,8 +6237,8 @@
       <c r="E106" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F106" s="69">
-        <v>10732.83102013364</v>
+      <c r="F106" s="68">
+        <v>10732.82974394128</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -6264,8 +6257,8 @@
       <c r="E107" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F107" s="69">
-        <v>10735.00084550465</v>
+      <c r="F107" s="68">
+        <v>10735.01111208054</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -6284,8 +6277,8 @@
       <c r="E108" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F108" s="69">
-        <v>10736.26251476708</v>
+      <c r="F108" s="68">
+        <v>10736.242387483</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -6304,8 +6297,8 @@
       <c r="E109" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F109" s="69">
-        <v>10737.18687700934</v>
+      <c r="F109" s="68">
+        <v>10737.19714358523</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -6324,8 +6317,8 @@
       <c r="E110" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F110" s="69">
-        <v>10732.65656593712</v>
+      <c r="F110" s="68">
+        <v>10732.65959946059</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -6344,8 +6337,8 @@
       <c r="E111" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F111" s="69">
-        <v>10732.47864172571</v>
+      <c r="F111" s="68">
+        <v>10732.47981876086</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -6364,8 +6357,8 @@
       <c r="E112" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F112" s="69">
-        <v>10732.94479684269</v>
+      <c r="F112" s="68">
+        <v>10732.94817607782</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -6384,8 +6377,8 @@
       <c r="E113" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F113" s="69">
-        <v>10733.64041016837</v>
+      <c r="F113" s="68">
+        <v>10733.64378940349</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -6404,7 +6397,7 @@
       <c r="E114" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F114" s="69">
+      <c r="F114" s="68">
         <v>10732.2656132467</v>
       </c>
     </row>
@@ -6424,7 +6417,7 @@
       <c r="E115" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F115" s="69">
+      <c r="F115" s="68">
         <v>10732.2656132467</v>
       </c>
     </row>
@@ -6444,7 +6437,7 @@
       <c r="E116" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F116" s="69">
+      <c r="F116" s="68">
         <v>10732.2656132467</v>
       </c>
     </row>
@@ -6464,7 +6457,7 @@
       <c r="E117" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F117" s="69">
+      <c r="F117" s="68">
         <v>10732.35593149356</v>
       </c>
     </row>
@@ -6484,7 +6477,7 @@
       <c r="E118" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F118" s="69">
+      <c r="F118" s="68">
         <v>10732.29701191123</v>
       </c>
     </row>
@@ -6504,7 +6497,7 @@
       <c r="E119" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F119" s="69">
+      <c r="F119" s="68">
         <v>10732.27401429305</v>
       </c>
     </row>
@@ -6524,7 +6517,7 @@
       <c r="E120" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F120" s="69">
+      <c r="F120" s="68">
         <v>10732.32859247224</v>
       </c>
     </row>
@@ -6544,7 +6537,7 @@
       <c r="E121" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F121" s="69">
+      <c r="F121" s="68">
         <v>10732.61398926761</v>
       </c>
     </row>
@@ -6564,8 +6557,8 @@
       <c r="E122" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F122" s="70">
-        <v>11013.38564421196</v>
+      <c r="F122" s="69">
+        <v>11015.35178058107</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -6584,8 +6577,8 @@
       <c r="E123" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F123" s="71">
-        <v>10379.00927871477</v>
+      <c r="F123" s="70">
+        <v>10380.69420387899</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -6604,8 +6597,8 @@
       <c r="E124" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F124" s="72">
-        <v>9944.605189503889</v>
+      <c r="F124" s="71">
+        <v>9946.187506781527</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -6624,8 +6617,8 @@
       <c r="E125" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F125" s="73">
-        <v>8901.755756938424</v>
+      <c r="F125" s="72">
+        <v>8903.250902653697</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -6644,8 +6637,8 @@
       <c r="E126" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F126" s="74">
-        <v>1088.706957395976</v>
+      <c r="F126" s="73">
+        <v>1088.718914850149</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -6664,8 +6657,8 @@
       <c r="E127" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F127" s="74">
-        <v>1074.091173717198</v>
+      <c r="F127" s="73">
+        <v>1074.103131171371</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -6684,8 +6677,8 @@
       <c r="E128" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F128" s="74">
-        <v>1083.501634142172</v>
+      <c r="F128" s="73">
+        <v>1083.566746473921</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -6704,8 +6697,8 @@
       <c r="E129" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F129" s="74">
-        <v>1064.823266510644</v>
+      <c r="F129" s="73">
+        <v>1064.83516248994</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -6724,8 +6717,8 @@
       <c r="E130" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F130" s="74">
-        <v>1074.361699410728</v>
+      <c r="F130" s="73">
+        <v>1074.372729382242</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -6744,8 +6737,8 @@
       <c r="E131" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F131" s="74">
-        <v>1079.309226807976</v>
+      <c r="F131" s="73">
+        <v>1079.352539398994</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -6764,8 +6757,8 @@
       <c r="E132" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F132" s="74">
-        <v>1072.442693700529</v>
+      <c r="F132" s="73">
+        <v>1072.486006291548</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -6784,8 +6777,8 @@
       <c r="E133" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F133" s="74">
-        <v>1071.830651882318</v>
+      <c r="F133" s="73">
+        <v>1071.873964473336</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -6804,8 +6797,8 @@
       <c r="E134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F134" s="74">
-        <v>1065.025175189018</v>
+      <c r="F134" s="73">
+        <v>1065.031819136754</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -6824,8 +6817,8 @@
       <c r="E135" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F135" s="74">
-        <v>1064.270740639324</v>
+      <c r="F135" s="73">
+        <v>1064.277384587059</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -6844,8 +6837,8 @@
       <c r="E136" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F136" s="74">
-        <v>1066.415588652227</v>
+      <c r="F136" s="73">
+        <v>1066.436087613017</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -6864,8 +6857,8 @@
       <c r="E137" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F137" s="74">
-        <v>1064.792831148335</v>
+      <c r="F137" s="73">
+        <v>1064.813330109125</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -6884,7 +6877,7 @@
       <c r="E138" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F138" s="74">
+      <c r="F138" s="73">
         <v>1059.060913223509</v>
       </c>
     </row>
@@ -6904,7 +6897,7 @@
       <c r="E139" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F139" s="74">
+      <c r="F139" s="73">
         <v>1059.060913223509</v>
       </c>
     </row>
@@ -6924,7 +6917,7 @@
       <c r="E140" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F140" s="74">
+      <c r="F140" s="73">
         <v>1059.060913223509</v>
       </c>
     </row>
@@ -6944,7 +6937,7 @@
       <c r="E141" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F141" s="74">
+      <c r="F141" s="73">
         <v>1059.304359890403</v>
       </c>
     </row>
@@ -6964,7 +6957,7 @@
       <c r="E142" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F142" s="74">
+      <c r="F142" s="73">
         <v>1059.57984840324</v>
       </c>
     </row>
@@ -6984,7 +6977,7 @@
       <c r="E143" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F143" s="74">
+      <c r="F143" s="73">
         <v>1059.484824320415</v>
       </c>
     </row>
@@ -7004,7 +6997,7 @@
       <c r="E144" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F144" s="74">
+      <c r="F144" s="73">
         <v>1059.364588033805</v>
       </c>
     </row>
@@ -7024,7 +7017,7 @@
       <c r="E145" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F145" s="74">
+      <c r="F145" s="73">
         <v>1059.205045511529</v>
       </c>
     </row>
@@ -7554,8 +7547,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="75">
-        <v>1192.566742520837</v>
+      <c r="F26" s="74">
+        <v>1190.152650121769</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7574,8 +7567,8 @@
       <c r="E27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="76">
-        <v>1630.643563649013</v>
+      <c r="F27" s="75">
+        <v>1628.371702917464</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7594,8 +7587,8 @@
       <c r="E28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="77">
-        <v>2042.330633151393</v>
+      <c r="F28" s="76">
+        <v>2040.226496212629</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7614,8 +7607,8 @@
       <c r="E29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="78">
-        <v>2482.267299117108</v>
+      <c r="F29" s="77">
+        <v>2480.564110501467</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7634,8 +7627,8 @@
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="79">
-        <v>3254.461263313218</v>
+      <c r="F30" s="78">
+        <v>3254.461085421613</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -7654,8 +7647,8 @@
       <c r="E31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="79">
-        <v>3265.814139372522</v>
+      <c r="F31" s="78">
+        <v>3265.813961480916</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -7674,8 +7667,8 @@
       <c r="E32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="79">
-        <v>3275.25079592668</v>
+      <c r="F32" s="78">
+        <v>3275.250768263941</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7694,8 +7687,8 @@
       <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="79">
-        <v>3281.045971137885</v>
+      <c r="F33" s="78">
+        <v>3281.045943475146</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -7714,8 +7707,8 @@
       <c r="E34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="80">
-        <v>3231.416386024011</v>
+      <c r="F34" s="79">
+        <v>3231.292671829926</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -7734,8 +7727,8 @@
       <c r="E35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="79">
-        <v>3250.055113761306</v>
+      <c r="F35" s="78">
+        <v>3249.93139956722</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -7754,8 +7747,8 @@
       <c r="E36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="79">
-        <v>3272.868885314663</v>
+      <c r="F36" s="78">
+        <v>3272.745171120578</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -7774,8 +7767,8 @@
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="79">
-        <v>3270.301141033458</v>
+      <c r="F37" s="78">
+        <v>3270.177426839373</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -7794,8 +7787,8 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="79">
-        <v>3260.578588627987</v>
+      <c r="F38" s="78">
+        <v>3260.508076661006</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -7814,8 +7807,8 @@
       <c r="E39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="79">
-        <v>3264.737840520364</v>
+      <c r="F39" s="78">
+        <v>3264.667328553383</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -7834,8 +7827,8 @@
       <c r="E40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="79">
-        <v>3254.695654522929</v>
+      <c r="F40" s="78">
+        <v>3254.517891401251</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -7854,8 +7847,8 @@
       <c r="E41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="79">
-        <v>3260.490829734134</v>
+      <c r="F41" s="78">
+        <v>3260.313066612457</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -7874,7 +7867,7 @@
       <c r="E42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="81">
+      <c r="F42" s="80">
         <v>3339.915892899608</v>
       </c>
     </row>
@@ -7894,7 +7887,7 @@
       <c r="E43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="81">
+      <c r="F43" s="80">
         <v>3339.915892899608</v>
       </c>
     </row>
@@ -7914,7 +7907,7 @@
       <c r="E44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="81">
+      <c r="F44" s="80">
         <v>3339.915892899608</v>
       </c>
     </row>
@@ -7934,8 +7927,8 @@
       <c r="E45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="79">
-        <v>3289.348094855413</v>
+      <c r="F45" s="78">
+        <v>3304.849255747775</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -7954,7 +7947,7 @@
       <c r="E46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="81">
+      <c r="F46" s="80">
         <v>3339.915892899608</v>
       </c>
     </row>
@@ -7974,7 +7967,7 @@
       <c r="E47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="81">
+      <c r="F47" s="80">
         <v>3332.665000212848</v>
       </c>
     </row>
@@ -7994,7 +7987,7 @@
       <c r="E48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="81">
+      <c r="F48" s="80">
         <v>3332.91146370401</v>
       </c>
     </row>
@@ -8014,7 +8007,7 @@
       <c r="E49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F49" s="81">
+      <c r="F49" s="80">
         <v>3334.200255151443</v>
       </c>
     </row>
@@ -8034,8 +8027,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="78">
-        <v>2481.024726476281</v>
+      <c r="F50" s="77">
+        <v>2477.634212148951</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -8054,8 +8047,8 @@
       <c r="E51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="82">
-        <v>3440.956080711199</v>
+      <c r="F51" s="81">
+        <v>3438.011684338143</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -8074,8 +8067,8 @@
       <c r="E52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="83">
-        <v>4085.274564466942</v>
+      <c r="F52" s="82">
+        <v>4082.462840033129</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -8094,8 +8087,8 @@
       <c r="E53" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="84">
-        <v>5339.354453251439</v>
+      <c r="F53" s="83">
+        <v>5336.833293919843</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -8115,7 +8108,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="43">
-        <v>14336.46364295511</v>
+        <v>14336.39511655654</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -8135,7 +8128,7 @@
         <v>16</v>
       </c>
       <c r="F55" s="43">
-        <v>14396.64852189639</v>
+        <v>14396.57999549782</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -8155,7 +8148,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="44">
-        <v>14467.4977514981</v>
+        <v>14467.42922509952</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -8175,7 +8168,7 @@
         <v>17</v>
       </c>
       <c r="F57" s="44">
-        <v>14423.37221738594</v>
+        <v>14423.30369098736</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -8195,7 +8188,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="44">
-        <v>14426.76509905753</v>
+        <v>14426.61552909569</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -8215,7 +8208,7 @@
         <v>16</v>
       </c>
       <c r="F59" s="44">
-        <v>14449.96513881417</v>
+        <v>14449.81556885234</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -8235,7 +8228,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="44">
-        <v>14478.38171960622</v>
+        <v>14478.23214964439</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -8255,7 +8248,7 @@
         <v>17</v>
       </c>
       <c r="F61" s="44">
-        <v>14475.9040845072</v>
+        <v>14475.75451454536</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -8275,7 +8268,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="40">
-        <v>14646.29085739002</v>
+        <v>14646.20348020904</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -8295,7 +8288,7 @@
         <v>16</v>
       </c>
       <c r="F63" s="40">
-        <v>14651.53274150672</v>
+        <v>14651.44536432575</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -8315,7 +8308,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="39">
-        <v>14578.68764784007</v>
+        <v>14578.46822815151</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -8335,7 +8328,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="39">
-        <v>14586.26866467298</v>
+        <v>14586.04924498442</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -8354,7 +8347,7 @@
       <c r="E66" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="85">
+      <c r="F66" s="84">
         <v>15078.75286938478</v>
       </c>
     </row>
@@ -8374,7 +8367,7 @@
       <c r="E67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="85">
+      <c r="F67" s="84">
         <v>15078.75286938478</v>
       </c>
     </row>
@@ -8394,7 +8387,7 @@
       <c r="E68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="85">
+      <c r="F68" s="84">
         <v>15078.75286938478</v>
       </c>
     </row>
@@ -8414,8 +8407,8 @@
       <c r="E69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F69" s="42">
-        <v>14813.83789795569</v>
+      <c r="F69" s="85">
+        <v>14892.88670034486</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -8434,7 +8427,7 @@
       <c r="E70" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F70" s="85">
+      <c r="F70" s="84">
         <v>15078.75286938478</v>
       </c>
     </row>
@@ -8995,7 +8988,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="87">
-        <v>1438.712105889249</v>
+        <v>1435.710155762264</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -9014,8 +9007,8 @@
       <c r="E99" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="77">
-        <v>2073.884421792527</v>
+      <c r="F99" s="76">
+        <v>2071.087232439284</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -9035,7 +9028,7 @@
         <v>13</v>
       </c>
       <c r="F100" s="88">
-        <v>2599.256408716236</v>
+        <v>2596.654884509274</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -9055,7 +9048,7 @@
         <v>17</v>
       </c>
       <c r="F101" s="89">
-        <v>3615.442374882401</v>
+        <v>3613.528657774847</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -9075,7 +9068,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="90">
-        <v>5254.658944831477</v>
+        <v>5254.658944806094</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -9115,7 +9108,7 @@
         <v>13</v>
       </c>
       <c r="F104" s="90">
-        <v>5253.927584194422</v>
+        <v>5253.771766873075</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -9155,7 +9148,7 @@
         <v>11</v>
       </c>
       <c r="F106" s="90">
-        <v>5254.658060928985</v>
+        <v>5254.658058053052</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -9175,7 +9168,7 @@
         <v>16</v>
       </c>
       <c r="F107" s="90">
-        <v>5251.200340626643</v>
+        <v>5251.1316946841</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -9215,7 +9208,7 @@
         <v>17</v>
       </c>
       <c r="F109" s="90">
-        <v>5253.30891996581</v>
+        <v>5253.240274023266</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -9235,7 +9228,7 @@
         <v>11</v>
       </c>
       <c r="F110" s="90">
-        <v>5253.217608320778</v>
+        <v>5253.204067140179</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -9255,7 +9248,7 @@
         <v>16</v>
       </c>
       <c r="F111" s="90">
-        <v>5254.33520328778</v>
+        <v>5254.325830229775</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -9275,7 +9268,7 @@
         <v>13</v>
       </c>
       <c r="F112" s="90">
-        <v>5253.634057135427</v>
+        <v>5253.605593798564</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -9295,7 +9288,7 @@
         <v>17</v>
       </c>
       <c r="F113" s="90">
-        <v>5254.317633437082</v>
+        <v>5254.289170100219</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -9475,7 +9468,7 @@
         <v>11</v>
       </c>
       <c r="F122" s="91">
-        <v>2381.273593248932</v>
+        <v>2376.942667200044</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -9495,7 +9488,7 @@
         <v>16</v>
       </c>
       <c r="F123" s="92">
-        <v>3832.21096861236</v>
+        <v>3828.470016198345</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -9515,7 +9508,7 @@
         <v>13</v>
       </c>
       <c r="F124" s="93">
-        <v>4865.777262699698</v>
+        <v>4862.252861316723</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -9535,7 +9528,7 @@
         <v>17</v>
       </c>
       <c r="F125" s="94">
-        <v>7119.320605000225</v>
+        <v>7115.980371353848</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -9554,8 +9547,8 @@
       <c r="E126" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F126" s="63">
-        <v>23578.91448068537</v>
+      <c r="F126" s="62">
+        <v>23578.88444452253</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -9574,8 +9567,8 @@
       <c r="E127" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F127" s="63">
-        <v>23615.70389965204</v>
+      <c r="F127" s="62">
+        <v>23615.6738634892</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -9594,8 +9587,8 @@
       <c r="E128" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F128" s="63">
-        <v>23600.98989112295</v>
+      <c r="F128" s="62">
+        <v>23600.81358492681</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -9614,8 +9607,8 @@
       <c r="E129" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F129" s="63">
-        <v>23639.63739126733</v>
+      <c r="F129" s="62">
+        <v>23639.60752562124</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -9634,8 +9627,8 @@
       <c r="E130" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F130" s="63">
-        <v>23615.00185378734</v>
+      <c r="F130" s="62">
+        <v>23614.97399550261</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -9654,8 +9647,8 @@
       <c r="E131" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F131" s="63">
-        <v>23602.46106931721</v>
+      <c r="F131" s="62">
+        <v>23602.35161186323</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -9674,8 +9667,8 @@
       <c r="E132" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F132" s="63">
-        <v>23619.77297051077</v>
+      <c r="F132" s="62">
+        <v>23619.66351305681</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -9694,8 +9687,8 @@
       <c r="E133" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F133" s="63">
-        <v>23621.89113974066</v>
+      <c r="F133" s="62">
+        <v>23621.78168228667</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -9714,8 +9707,8 @@
       <c r="E134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F134" s="63">
-        <v>23638.58114996401</v>
+      <c r="F134" s="62">
+        <v>23638.56454010699</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -9734,8 +9727,8 @@
       <c r="E135" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F135" s="63">
-        <v>23640.46418243904</v>
+      <c r="F135" s="62">
+        <v>23640.44757258202</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -9754,8 +9747,8 @@
       <c r="E136" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F136" s="63">
-        <v>23635.05738166095</v>
+      <c r="F136" s="62">
+        <v>23635.0059516591</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -9774,8 +9767,8 @@
       <c r="E137" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F137" s="63">
-        <v>23639.72202872111</v>
+      <c r="F137" s="62">
+        <v>23639.67059871925</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -9794,7 +9787,7 @@
       <c r="E138" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F138" s="63">
+      <c r="F138" s="62">
         <v>23653.46811738121</v>
       </c>
     </row>
@@ -9814,7 +9807,7 @@
       <c r="E139" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F139" s="63">
+      <c r="F139" s="62">
         <v>23653.46811738121</v>
       </c>
     </row>
@@ -9834,7 +9827,7 @@
       <c r="E140" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F140" s="63">
+      <c r="F140" s="62">
         <v>23653.46811738121</v>
       </c>
     </row>
@@ -9854,7 +9847,7 @@
       <c r="E141" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F141" s="63">
+      <c r="F141" s="62">
         <v>23652.86218633332</v>
       </c>
     </row>
@@ -9874,7 +9867,7 @@
       <c r="E142" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F142" s="63">
+      <c r="F142" s="62">
         <v>23652.17650414513</v>
       </c>
     </row>
@@ -9894,7 +9887,7 @@
       <c r="E143" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F143" s="63">
+      <c r="F143" s="62">
         <v>23652.41301607941</v>
       </c>
     </row>
@@ -9914,7 +9907,7 @@
       <c r="E144" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F144" s="63">
+      <c r="F144" s="62">
         <v>23652.71228039084</v>
       </c>
     </row>
@@ -9934,7 +9927,7 @@
       <c r="E145" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F145" s="63">
+      <c r="F145" s="62">
         <v>23653.46811738121</v>
       </c>
     </row>
@@ -9985,7 +9978,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="95">
-        <v>891.6379243396411</v>
+        <v>890.0308285183272</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -10005,7 +9998,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="96">
-        <v>1497.619539848368</v>
+        <v>1496.012444027054</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -10025,7 +10018,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="97">
-        <v>2108.852134669048</v>
+        <v>2107.245038847735</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -10045,7 +10038,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="38">
-        <v>2798.420313221865</v>
+        <v>2796.81321740055</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -10065,7 +10058,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="98">
-        <v>83.67070784214913</v>
+        <v>83.61744168785674</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -10085,7 +10078,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="9">
-        <v>125.1019419704355</v>
+        <v>125.0486758161432</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -10105,7 +10098,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="11">
-        <v>173.5485212627592</v>
+        <v>173.4952551084668</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -10125,7 +10118,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="99">
-        <v>135.8697746539861</v>
+        <v>135.8165084996937</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -10145,7 +10138,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="8">
-        <v>23.47411535832032</v>
+        <v>23.36142772050749</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -10165,7 +10158,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="100">
-        <v>39.28710372161073</v>
+        <v>39.17441608379789</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -10185,7 +10178,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="101">
-        <v>58.59865710497272</v>
+        <v>58.48596946715987</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -10205,7 +10198,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="102">
-        <v>53.2821589512056</v>
+        <v>53.16947131339276</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -10225,7 +10218,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="7">
-        <v>3.750481165757633</v>
+        <v>3.725005432296051</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -10245,7 +10238,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="7">
-        <v>7.159963423009469</v>
+        <v>7.096133090591663</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -10265,7 +10258,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="7">
-        <v>12.22159626906361</v>
+        <v>12.06095479092581</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -10285,7 +10278,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="7">
-        <v>16.00287671280401</v>
+        <v>15.93904638038621</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -10365,7 +10358,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="7">
-        <v>0.6203965791365842</v>
+        <v>0.4616302094927468</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -10465,7 +10458,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="103">
-        <v>316.308523608446</v>
+        <v>316.0915251485631</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -10485,7 +10478,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="29">
-        <v>654.2233464420679</v>
+        <v>653.9542425013495</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -10505,7 +10498,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="104">
-        <v>1006.211821733541</v>
+        <v>1005.87961023689</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -10525,7 +10518,7 @@
         <v>17</v>
       </c>
       <c r="F29" s="22">
-        <v>1442.157762366012</v>
+        <v>1441.670002341504</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -10545,7 +10538,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="7">
-        <v>6.343992701790799</v>
+        <v>6.290866738551616</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -10565,7 +10558,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="100">
-        <v>40.6996067061246</v>
+        <v>40.64648060802619</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -10585,7 +10578,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="98">
-        <v>84.16242741010024</v>
+        <v>84.10917964739554</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -10605,7 +10598,7 @@
         <v>17</v>
       </c>
       <c r="F33" s="102">
-        <v>45.24202376386208</v>
+        <v>45.18877600115736</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -10965,7 +10958,7 @@
         <v>16</v>
       </c>
       <c r="F51" s="10">
-        <v>194.8436842875938</v>
+        <v>194.7112420316693</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -10985,7 +10978,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="105">
-        <v>489.0984688633728</v>
+        <v>488.9257397876959</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -11005,7 +10998,7 @@
         <v>17</v>
       </c>
       <c r="F53" s="29">
-        <v>662.5212657185186</v>
+        <v>662.2544729695388</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -11425,7 +11418,7 @@
         <v>11</v>
       </c>
       <c r="F74" s="95">
-        <v>889.5581793048835</v>
+        <v>887.748580684791</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -11444,8 +11437,8 @@
       <c r="E75" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F75" s="106">
-        <v>1495.539794813611</v>
+      <c r="F75" s="96">
+        <v>1493.730196193518</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -11465,7 +11458,7 @@
         <v>13</v>
       </c>
       <c r="F76" s="97">
-        <v>2106.772389634291</v>
+        <v>2104.962791014199</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -11485,7 +11478,7 @@
         <v>17</v>
       </c>
       <c r="F77" s="38">
-        <v>2796.340568187108</v>
+        <v>2794.530969567015</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -11505,7 +11498,7 @@
         <v>11</v>
       </c>
       <c r="F78" s="101">
-        <v>60.09835598885094</v>
+        <v>60.07463586395637</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -11525,7 +11518,7 @@
         <v>16</v>
       </c>
       <c r="F79" s="98">
-        <v>85.85168833488918</v>
+        <v>85.82796820999462</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -11545,7 +11538,7 @@
         <v>13</v>
       </c>
       <c r="F80" s="9">
-        <v>126.4091673539462</v>
+        <v>126.2431982309678</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -11564,8 +11557,8 @@
       <c r="E81" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F81" s="107">
-        <v>99.29466065028961</v>
+      <c r="F81" s="106">
+        <v>99.27094052539503</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -11585,7 +11578,7 @@
         <v>11</v>
       </c>
       <c r="F82" s="7">
-        <v>12.90929501766869</v>
+        <v>12.88811012301628</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -11605,7 +11598,7 @@
         <v>16</v>
       </c>
       <c r="F83" s="7">
-        <v>19.96795399733703</v>
+        <v>19.88410073908514</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -11625,7 +11618,7 @@
         <v>13</v>
       </c>
       <c r="F84" s="8">
-        <v>31.90577197617944</v>
+        <v>31.82191871792756</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -11645,7 +11638,7 @@
         <v>17</v>
       </c>
       <c r="F85" s="100">
-        <v>32.87485413930497</v>
+        <v>32.79100088105308</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -11665,7 +11658,7 @@
         <v>11</v>
       </c>
       <c r="F86" s="7">
-        <v>2.088454415073838</v>
+        <v>2.076092826937894</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -11685,7 +11678,7 @@
         <v>16</v>
       </c>
       <c r="F87" s="7">
-        <v>3.401887905764125</v>
+        <v>3.389526317628182</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -11705,7 +11698,7 @@
         <v>13</v>
       </c>
       <c r="F88" s="7">
-        <v>5.687780470070891</v>
+        <v>5.649434086945375</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -11725,7 +11718,7 @@
         <v>17</v>
       </c>
       <c r="F89" s="7">
-        <v>9.811447179867596</v>
+        <v>9.77310079674208</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -11905,7 +11898,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="13">
-        <v>224.7675736056675</v>
+        <v>224.4709615808381</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -11924,8 +11917,8 @@
       <c r="E99" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="108">
-        <v>493.7026031928395</v>
+      <c r="F99" s="107">
+        <v>493.3405424421207</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -11944,8 +11937,8 @@
       <c r="E100" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F100" s="109">
-        <v>805.2088898270712</v>
+      <c r="F100" s="108">
+        <v>804.7745864116532</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -11964,8 +11957,8 @@
       <c r="E101" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F101" s="110">
-        <v>1021.158581048332</v>
+      <c r="F101" s="109">
+        <v>1020.473655640766</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -11985,7 +11978,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="8">
-        <v>29.8951965027391</v>
+        <v>29.8714763804514</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -12005,7 +11998,7 @@
         <v>16</v>
       </c>
       <c r="F103" s="101">
-        <v>55.64700766200211</v>
+        <v>55.62328753710755</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -12025,7 +12018,7 @@
         <v>13</v>
       </c>
       <c r="F104" s="98">
-        <v>86.51877795413894</v>
+        <v>86.49505782924437</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -12044,8 +12037,8 @@
       <c r="E105" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F105" s="111">
-        <v>69.08997997740256</v>
+      <c r="F105" s="110">
+        <v>69.06625985250801</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -12065,7 +12058,7 @@
         <v>11</v>
       </c>
       <c r="F106" s="7">
-        <v>2.321555727683656</v>
+        <v>2.316278604380043</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -12085,7 +12078,7 @@
         <v>16</v>
       </c>
       <c r="F107" s="7">
-        <v>8.09284440244744</v>
+        <v>8.071659507795037</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -12105,7 +12098,7 @@
         <v>13</v>
       </c>
       <c r="F108" s="7">
-        <v>16.53915466293458</v>
+        <v>16.45530140468269</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -12125,7 +12118,7 @@
         <v>17</v>
       </c>
       <c r="F109" s="7">
-        <v>19.07477692347624</v>
+        <v>19.05359202882384</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -12165,7 +12158,7 @@
         <v>16</v>
       </c>
       <c r="F111" s="7">
-        <v>0.5668855977053042</v>
+        <v>0.563080876667762</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -12185,7 +12178,7 @@
         <v>13</v>
       </c>
       <c r="F112" s="7">
-        <v>1.841359745926942</v>
+        <v>1.828998157790998</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -12205,7 +12198,7 @@
         <v>17</v>
       </c>
       <c r="F113" s="7">
-        <v>5.340974885699489</v>
+        <v>5.328613297563545</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -12405,7 +12398,7 @@
         <v>16</v>
       </c>
       <c r="F123" s="102">
-        <v>46.14691150178646</v>
+        <v>45.97362802507425</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -12425,7 +12418,7 @@
         <v>13</v>
       </c>
       <c r="F124" s="13">
-        <v>220.3025001370114</v>
+        <v>220.0654997115531</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -12445,7 +12438,7 @@
         <v>17</v>
       </c>
       <c r="F125" s="98">
-        <v>84.21790120316125</v>
+        <v>83.924781096443</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -12505,7 +12498,7 @@
         <v>13</v>
       </c>
       <c r="F128" s="7">
-        <v>14.57403294782393</v>
+        <v>14.55036203084586</v>
       </c>
     </row>
     <row r="129" spans="1:6">

</xml_diff>

<commit_message>
Fixed V2G capacity bug
</commit_message>
<xml_diff>
--- a/results/Manuscript/material_use.xlsx
+++ b/results/Manuscript/material_use.xlsx
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="81">
+  <fills count="122">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,13 +120,625 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4DFDF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C7C7"/>
+        <fgColor rgb="FFF4E0E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C8C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B9B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E4E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DBDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3ECEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EFEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5CBCB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5BEBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6AAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF89090"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EBEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C4C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E9E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB4848"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3939"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF96F6F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6868"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97171"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97070"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB4949"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3B3B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6969"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA5F5F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97272"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB4C4C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD2121"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF96E6E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FC68F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8CC58C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BC48B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DC58D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90C790"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BCC9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2CFA2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6D2A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91C791"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95C995"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8DAB8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1E6D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF3EB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98CA98"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0CEA0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCDCBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF97CA97"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF038103"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF058205"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF068306"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF138913"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1D8E1D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF289328"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF128912"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E972E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF56AA56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7CBD7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF098509"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF148A14"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF319831"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF088408"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF078407"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC2DFC2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3D0A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92C892"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6F1E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3EFE3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3E7D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F1E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9ECE9E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF69B369"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF349A34"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDECDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9E2C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCECDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFEDDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DB66D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EEE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBDCBB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAF2EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4AA44A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCBE4CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5F0E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7A3A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3A3A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6ABAB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF88B8B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D5D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E1E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E8E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DEDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79B9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97777"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,49 +750,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3EFEF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EEEE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5CACA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5BDBD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5CBCB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6A9A9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF88F8F"/>
+        <fgColor rgb="FFF6ACAC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,355 +762,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA6060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4848"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC3939"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97070"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF96F6F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97171"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97272"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA5F5F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4949"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC3A3A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4B4B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFD2121"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8FC68F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8CC58C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8BC48B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90C790"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF91C791"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BCC9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA2CFA2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA6D2A6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8DAB8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1E6D1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF3EB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94C994"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF038103"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF058205"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF068306"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF138913"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1D8E1D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF289328"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2E972E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF56AA56"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CBD7C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF088408"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF078407"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC2DFC2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA3D0A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92C892"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEAF2EA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ECE9E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF69B369"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF349A34"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7F1E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5F0E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6DB66D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4AA44A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2E8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6F1E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7A3A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E9E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4E2E2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E6E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D5D5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79B9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97777"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E8E8"/>
+        <fgColor rgb="FFF3E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E5E5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,13 +792,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3EBEB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E8E7"/>
+        <fgColor rgb="FFF4D6D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E3E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79F9F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,13 +822,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6ABAB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF79898"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D0D0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -638,12 +884,12 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -651,51 +897,51 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -705,6 +951,47 @@
     <xf numFmtId="0" fontId="2" fillId="78" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="79" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="80" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="81" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="82" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="83" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="84" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="85" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="90" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="91" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="92" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="93" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="94" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="95" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="96" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="97" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="98" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="99" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="100" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="102" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="103" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="104" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="105" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="106" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="109" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="110" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="111" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="112" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="113" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="114" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="115" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="116" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="117" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="118" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="119" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="120" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="121" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="6">
-        <v>37383.15159403763</v>
+        <v>37490.49492452692</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1119,7 +1406,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="7">
-        <v>37441.13681757262</v>
+        <v>37887.56661130874</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1138,8 +1425,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="7">
-        <v>37416.69826644933</v>
+      <c r="F7" s="8">
+        <v>38212.80964096187</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1158,8 +1445,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8">
-        <v>37334.97167483041</v>
+      <c r="F8" s="9">
+        <v>37385.76194420527</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1178,8 +1465,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="8">
-        <v>37339.27911170072</v>
+      <c r="F9" s="10">
+        <v>37545.99352427768</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1198,8 +1485,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="8">
-        <v>37342.05625162341</v>
+      <c r="F10" s="11">
+        <v>37453.02879417115</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1218,8 +1505,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="8">
-        <v>37332.79195938796</v>
+      <c r="F11" s="9">
+        <v>37395.54083966072</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1238,8 +1525,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="8">
-        <v>37332.79195938796</v>
+      <c r="F12" s="10">
+        <v>37559.4511818316</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1258,8 +1545,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8">
-        <v>37333.32604654493</v>
+      <c r="F13" s="6">
+        <v>37472.21420633512</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1298,7 +1585,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="12">
         <v>38862.37038121407</v>
       </c>
     </row>
@@ -1318,7 +1605,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="13">
         <v>39409.03516301885</v>
       </c>
     </row>
@@ -1339,7 +1626,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="6">
-        <v>37377.18358916603</v>
+        <v>37483.88802480543</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1359,7 +1646,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="7">
-        <v>37435.16881270102</v>
+        <v>37872.04289509112</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1378,8 +1665,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="7">
-        <v>37410.73026157772</v>
+      <c r="F19" s="14">
+        <v>38189.8711056198</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1398,8 +1685,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="8">
-        <v>37334.33002438084</v>
+      <c r="F20" s="9">
+        <v>37379.58649703812</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1418,8 +1705,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="8">
-        <v>37337.85352696716</v>
+      <c r="F21" s="10">
+        <v>37537.94697893425</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1438,8 +1725,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="8">
-        <v>37340.57635823706</v>
+      <c r="F22" s="11">
+        <v>37448.19082480113</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1458,8 +1745,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="8">
-        <v>37332.79195938796</v>
+      <c r="F23" s="9">
+        <v>37389.50869071848</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1478,8 +1765,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="8">
-        <v>37332.79195938796</v>
+      <c r="F24" s="10">
+        <v>37552.30761756487</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1498,8 +1785,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="8">
-        <v>37333.29334855909</v>
+      <c r="F25" s="6">
+        <v>37463.17788648279</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1518,7 +1805,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="15">
         <v>38820.09493073855</v>
       </c>
     </row>
@@ -1538,7 +1825,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="16">
         <v>40176.08684177568</v>
       </c>
     </row>
@@ -1558,7 +1845,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="17">
         <v>41241.89777610592</v>
       </c>
     </row>
@@ -1578,8 +1865,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="6">
-        <v>37404.04639626412</v>
+      <c r="F29" s="18">
+        <v>37603.96999706588</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1599,7 +1886,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="14">
-        <v>37474.5840367792</v>
+        <v>38186.62819753488</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1618,8 +1905,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="14">
-        <v>37451.94694363237</v>
+      <c r="F31" s="19">
+        <v>39170.48945010785</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1638,8 +1925,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="8">
-        <v>37335.78573278843</v>
+      <c r="F32" s="9">
+        <v>37411.42027899526</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1658,8 +1945,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="8">
-        <v>37341.6846714218</v>
+      <c r="F33" s="20">
+        <v>37648.1056894984</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1678,8 +1965,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="8">
-        <v>37345.30556767998</v>
+      <c r="F34" s="10">
+        <v>37564.1745709563</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1698,8 +1985,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="8">
-        <v>37332.79195938796</v>
+      <c r="F35" s="11">
+        <v>37427.75303016329</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1718,8 +2005,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="8">
-        <v>37332.79195938796</v>
+      <c r="F36" s="20">
+        <v>37658.53375115538</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1738,8 +2025,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="8">
-        <v>37333.36451097934</v>
+      <c r="F37" s="10">
+        <v>37561.84975887099</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1758,7 +2045,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="21">
         <v>43146.87751981514</v>
       </c>
     </row>
@@ -1778,7 +2065,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="22">
         <v>44101.76903663111</v>
       </c>
     </row>
@@ -1798,7 +2085,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="23">
         <v>44694.68505036762</v>
       </c>
     </row>
@@ -1818,8 +2105,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="18">
-        <v>42475.32805651157</v>
+      <c r="F41" s="24">
+        <v>42541.9678382339</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1838,8 +2125,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="19">
-        <v>42517.8453471593</v>
+      <c r="F42" s="25">
+        <v>42821.7152006235</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1858,8 +2145,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="18">
-        <v>42500.39894580901</v>
+      <c r="F43" s="21">
+        <v>43155.50989436005</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1878,8 +2165,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="20">
-        <v>42438.17707060384</v>
+      <c r="F44" s="26">
+        <v>42460.78688361657</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1898,8 +2185,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="20">
-        <v>42440.44808599587</v>
+      <c r="F45" s="27">
+        <v>42511.77039385081</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1918,8 +2205,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="20">
-        <v>42443.06928298871</v>
+      <c r="F46" s="26">
+        <v>42486.90840482202</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1938,8 +2225,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="21">
-        <v>42436.85760197356</v>
+      <c r="F47" s="26">
+        <v>42463.42532364777</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1958,8 +2245,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="21">
-        <v>42436.85760197356</v>
+      <c r="F48" s="24">
+        <v>42535.51332075584</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1978,8 +2265,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="21">
-        <v>42437.26270577266</v>
+      <c r="F49" s="26">
+        <v>42496.8518929108</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1998,7 +2285,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="22">
+      <c r="F50" s="21">
         <v>43174.29827220868</v>
       </c>
     </row>
@@ -2018,7 +2305,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="28">
         <v>44042.88994517744</v>
       </c>
     </row>
@@ -2038,7 +2325,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="24">
+      <c r="F52" s="29">
         <v>44632.76660394678</v>
       </c>
     </row>
@@ -2058,8 +2345,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="20">
-        <v>42469.6983827214</v>
+      <c r="F53" s="27">
+        <v>42529.41815279475</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2078,8 +2365,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="18">
-        <v>42511.08602923178</v>
+      <c r="F54" s="30">
+        <v>42792.54578025143</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2098,8 +2385,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="18">
-        <v>42494.76927201885</v>
+      <c r="F55" s="31">
+        <v>43207.54276501382</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2118,8 +2405,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="20">
-        <v>42437.85878947384</v>
+      <c r="F56" s="32">
+        <v>42456.26732785177</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2138,8 +2425,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="20">
-        <v>42439.84392065355</v>
+      <c r="F57" s="27">
+        <v>42505.64278778723</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2158,8 +2445,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="20">
-        <v>42442.3180540411</v>
+      <c r="F58" s="26">
+        <v>42481.97457043862</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2178,8 +2465,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="21">
-        <v>42436.85760197356</v>
+      <c r="F59" s="32">
+        <v>42458.78580147695</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2198,8 +2485,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="21">
-        <v>42436.85760197356</v>
+      <c r="F60" s="27">
+        <v>42525.5570406761</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2218,8 +2505,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="21">
-        <v>42437.24270872962</v>
+      <c r="F61" s="26">
+        <v>42489.3349762876</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2238,7 +2525,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="25">
+      <c r="F62" s="33">
         <v>43964.38010005821</v>
       </c>
     </row>
@@ -2258,7 +2545,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="26">
+      <c r="F63" s="34">
         <v>45673.59602566905</v>
       </c>
     </row>
@@ -2278,7 +2565,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="27">
+      <c r="F64" s="35">
         <v>47012.52701914091</v>
       </c>
     </row>
@@ -2298,8 +2585,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="18">
-        <v>42488.11400787481</v>
+      <c r="F65" s="36">
+        <v>42585.87510575628</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2318,8 +2605,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="19">
-        <v>42546.53978523452</v>
+      <c r="F66" s="37">
+        <v>43080.9108578156</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2338,8 +2625,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="19">
-        <v>42522.54561892624</v>
+      <c r="F67" s="28">
+        <v>44073.93921209701</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2358,8 +2645,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="20">
-        <v>42438.52127402808</v>
+      <c r="F68" s="26">
+        <v>42470.65558151645</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2378,8 +2665,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="20">
-        <v>42441.47084454677</v>
+      <c r="F69" s="24">
+        <v>42548.68478832724</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2398,8 +2685,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="20">
-        <v>42444.50156695934</v>
+      <c r="F70" s="27">
+        <v>42511.98215560726</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2418,8 +2705,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="21">
-        <v>42436.85760197356</v>
+      <c r="F71" s="26">
+        <v>42476.01538714891</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2438,8 +2725,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="21">
-        <v>42436.85760197356</v>
+      <c r="F72" s="36">
+        <v>42576.14125782856</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2458,8 +2745,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="21">
-        <v>42437.2854784107</v>
+      <c r="F73" s="27">
+        <v>42524.91536581161</v>
       </c>
     </row>
   </sheetData>
@@ -2508,7 +2795,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="38">
         <v>7526.317007325268</v>
       </c>
     </row>
@@ -2528,7 +2815,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="39">
         <v>7641.74377550096</v>
       </c>
     </row>
@@ -2548,7 +2835,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="40">
         <v>7655.177428068251</v>
       </c>
     </row>
@@ -2568,8 +2855,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="31">
-        <v>7451.716828000943</v>
+      <c r="F5" s="38">
+        <v>7484.587833051628</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2588,8 +2875,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="28">
-        <v>7472.76277769972</v>
+      <c r="F6" s="41">
+        <v>7585.895685811509</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2608,8 +2895,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="31">
-        <v>7464.069731189082</v>
+      <c r="F7" s="41">
+        <v>7592.270696098678</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2628,8 +2915,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="32">
-        <v>7433.99114782884</v>
+      <c r="F8" s="42">
+        <v>7452.407487892349</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2648,8 +2935,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="31">
-        <v>7435.640122759289</v>
+      <c r="F9" s="38">
+        <v>7504.132681232119</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2668,8 +2955,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="31">
-        <v>7436.704502746343</v>
+      <c r="F10" s="38">
+        <v>7475.121380337516</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2688,8 +2975,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="32">
-        <v>7433.155650036493</v>
+      <c r="F11" s="42">
+        <v>7455.714864070796</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2708,8 +2995,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="32">
-        <v>7433.155650036493</v>
+      <c r="F12" s="38">
+        <v>7508.886192690064</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2728,8 +3015,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="32">
-        <v>7433.360486766105</v>
+      <c r="F13" s="38">
+        <v>7481.233153766711</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2748,7 +3035,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="43">
         <v>7024.441944697281</v>
       </c>
     </row>
@@ -2768,7 +3055,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="44">
         <v>6783.149043639318</v>
       </c>
     </row>
@@ -2788,7 +3075,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="45">
         <v>6608.194684521932</v>
       </c>
     </row>
@@ -2808,8 +3095,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="32">
-        <v>7424.126568428437</v>
+      <c r="F17" s="46">
+        <v>7414.14403284752</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2828,8 +3115,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="31">
-        <v>7445.172518127214</v>
+      <c r="F18" s="42">
+        <v>7466.051404946031</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2848,8 +3135,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="31">
-        <v>7436.479471616576</v>
+      <c r="F19" s="47">
+        <v>7281.461323232128</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2868,8 +3155,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="32">
-        <v>7432.088028617432</v>
+      <c r="F20" s="46">
+        <v>7417.942739344348</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2888,8 +3175,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="32">
-        <v>7431.157890070519</v>
+      <c r="F21" s="42">
+        <v>7441.081573799078</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2908,8 +3195,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="32">
-        <v>7432.061072893499</v>
+      <c r="F22" s="46">
+        <v>7419.020354366328</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2928,8 +3215,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="32">
-        <v>7433.155650036493</v>
+      <c r="F23" s="46">
+        <v>7419.599452745066</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2948,8 +3235,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="32">
-        <v>7433.155650036493</v>
+      <c r="F24" s="42">
+        <v>7452.515101813799</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2968,8 +3255,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="32">
-        <v>7433.290842887682</v>
+      <c r="F25" s="46">
+        <v>7426.75481847604</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2988,7 +3275,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="48">
         <v>5972.38224728867</v>
       </c>
     </row>
@@ -3008,7 +3295,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="49">
         <v>5037.127154289265</v>
       </c>
     </row>
@@ -3028,7 +3315,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="38">
+      <c r="F28" s="50">
         <v>4035.335950068962</v>
       </c>
     </row>
@@ -3048,8 +3335,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="39">
-        <v>7361.901213160338</v>
+      <c r="F29" s="51">
+        <v>7165.596640501826</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3068,8 +3355,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="40">
-        <v>7326.551254751211</v>
+      <c r="F30" s="52">
+        <v>6853.464875756896</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3088,8 +3375,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="40">
-        <v>7321.544209534009</v>
+      <c r="F31" s="53">
+        <v>5805.453599291333</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3108,8 +3395,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="32">
-        <v>7430.161876636023</v>
+      <c r="F32" s="54">
+        <v>7354.527330429212</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3128,8 +3415,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="32">
-        <v>7424.58235250596</v>
+      <c r="F33" s="51">
+        <v>7175.401097826402</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3148,8 +3435,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="32">
-        <v>7421.996031435281</v>
+      <c r="F34" s="55">
+        <v>7203.138391749419</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3168,8 +3455,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="32">
-        <v>7433.155650036493</v>
+      <c r="F35" s="54">
+        <v>7338.194579261172</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3188,8 +3475,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="32">
-        <v>7433.155650036493</v>
+      <c r="F36" s="51">
+        <v>7187.485295646615</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3208,8 +3495,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="32">
-        <v>7432.816761687757</v>
+      <c r="F37" s="55">
+        <v>7209.490293436837</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3228,7 +3515,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="56">
         <v>12788.24710269182</v>
       </c>
     </row>
@@ -3248,7 +3535,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="42">
+      <c r="F39" s="57">
         <v>12903.67387086751</v>
       </c>
     </row>
@@ -3268,7 +3555,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="42">
+      <c r="F40" s="57">
         <v>12917.1075234348</v>
       </c>
     </row>
@@ -3288,8 +3575,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="43">
-        <v>12709.4366631453</v>
+      <c r="F41" s="58">
+        <v>12731.7596156854</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3308,8 +3595,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="43">
-        <v>12725.0847960323</v>
+      <c r="F42" s="56">
+        <v>12810.89635625786</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3328,8 +3615,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="43">
-        <v>12718.83178749379</v>
+      <c r="F43" s="56">
+        <v>12811.32360872874</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3348,8 +3635,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="44">
-        <v>12695.59169252209</v>
+      <c r="F44" s="59">
+        <v>12704.08076427906</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3368,8 +3655,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="44">
-        <v>12696.46212672706</v>
+      <c r="F45" s="58">
+        <v>12722.67516056393</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3388,8 +3675,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="44">
-        <v>12697.4669438271</v>
+      <c r="F46" s="58">
+        <v>12713.84252576112</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3408,8 +3695,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="44">
-        <v>12695.08574540304</v>
+      <c r="F47" s="59">
+        <v>12705.02792222194</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3428,8 +3715,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="44">
-        <v>12695.08574540304</v>
+      <c r="F48" s="58">
+        <v>12730.72059778032</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3448,8 +3735,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="44">
-        <v>12695.24111356024</v>
+      <c r="F49" s="58">
+        <v>12717.33891322959</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3468,7 +3755,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="45">
+      <c r="F50" s="60">
         <v>12160.95364948288</v>
       </c>
     </row>
@@ -3488,7 +3775,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="46">
+      <c r="F51" s="61">
         <v>11804.55485389116</v>
       </c>
     </row>
@@ -3508,7 +3795,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="47">
+      <c r="F52" s="62">
         <v>11407.37915216324</v>
       </c>
     </row>
@@ -3528,8 +3815,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="44">
-        <v>12689.30584990843</v>
+      <c r="F53" s="59">
+        <v>12679.70016894025</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3548,8 +3835,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="44">
-        <v>12697.70967167771</v>
+      <c r="F54" s="59">
+        <v>12672.15439138942</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3568,8 +3855,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="44">
-        <v>12698.70097425691</v>
+      <c r="F55" s="63">
+        <v>12201.70218765849</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3588,8 +3875,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="44">
-        <v>12694.75005632926</v>
+      <c r="F56" s="59">
+        <v>12686.19667243494</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3608,8 +3895,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="44">
-        <v>12694.76349296113</v>
+      <c r="F57" s="59">
+        <v>12692.50046340397</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3628,8 +3915,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="44">
-        <v>12695.36663392901</v>
+      <c r="F58" s="59">
+        <v>12691.5986040759</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3648,8 +3935,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="44">
-        <v>12695.08574540304</v>
+      <c r="F59" s="59">
+        <v>12683.90695736571</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3668,8 +3955,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="44">
-        <v>12695.08574540304</v>
+      <c r="F60" s="59">
+        <v>12691.98577033498</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3688,8 +3975,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="44">
-        <v>12695.19768260522</v>
+      <c r="F61" s="59">
+        <v>12689.11655282692</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3708,7 +3995,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="48">
+      <c r="F62" s="64">
         <v>11167.74671002897</v>
       </c>
     </row>
@@ -3728,7 +4015,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="49">
+      <c r="F63" s="65">
         <v>9657.024318165388</v>
       </c>
     </row>
@@ -3748,7 +4035,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="50">
+      <c r="F64" s="66">
         <v>8199.379735498071</v>
       </c>
     </row>
@@ -3768,8 +4055,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="44">
-        <v>12644.01280068436</v>
+      <c r="F65" s="67">
+        <v>12546.25170428193</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3788,8 +4075,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="51">
-        <v>12599.25009329226</v>
+      <c r="F66" s="68">
+        <v>12132.32622636768</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3808,8 +4095,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="52">
-        <v>12611.71872792113</v>
+      <c r="F67" s="69">
+        <v>11071.31079476583</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3828,8 +4115,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="44">
-        <v>12693.5919457478</v>
+      <c r="F68" s="59">
+        <v>12661.47079313621</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3848,8 +4135,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="44">
-        <v>12690.99658499857</v>
+      <c r="F69" s="70">
+        <v>12583.79579609485</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3868,8 +4155,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="44">
-        <v>12689.41610883089</v>
+      <c r="F70" s="71">
+        <v>12622.21903611022</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3888,8 +4175,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="44">
-        <v>12695.08574540304</v>
+      <c r="F71" s="59">
+        <v>12656.0694338469</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3908,8 +4195,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="44">
-        <v>12695.08574540304</v>
+      <c r="F72" s="67">
+        <v>12556.2977729367</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3928,8 +4215,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="44">
-        <v>12694.91959852269</v>
+      <c r="F73" s="71">
+        <v>12609.00118558295</v>
       </c>
     </row>
   </sheetData>
@@ -3978,7 +4265,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="50">
         <v>0</v>
       </c>
     </row>
@@ -3998,7 +4285,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4018,7 +4305,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4038,7 +4325,7 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4058,7 +4345,7 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4078,7 +4365,7 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4098,7 +4385,7 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4118,7 +4405,7 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4138,7 +4425,7 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4158,7 +4445,7 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4178,7 +4465,7 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4198,7 +4485,7 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4218,7 +4505,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="72">
         <v>1650.829858861342</v>
       </c>
     </row>
@@ -4238,7 +4525,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="73">
         <v>2881.854852240659</v>
       </c>
     </row>
@@ -4258,7 +4545,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="74">
         <v>3533.499652148049</v>
       </c>
     </row>
@@ -4278,8 +4565,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="56">
-        <v>66.26411867391265</v>
+      <c r="F17" s="75">
+        <v>183.827075772615</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4298,8 +4585,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="56">
-        <v>66.26411867391265</v>
+      <c r="F18" s="76">
+        <v>330.513716496191</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4318,8 +4605,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="56">
-        <v>66.26411867391265</v>
+      <c r="F19" s="77">
+        <v>976.3257276115362</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4338,8 +4625,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="38">
-        <v>4.610719237216883</v>
+      <c r="F20" s="78">
+        <v>84.24558607264686</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4358,8 +4645,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="38">
-        <v>10.6908626451255</v>
+      <c r="F21" s="79">
+        <v>161.7408486386202</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4378,8 +4665,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="38">
-        <v>11.06159656496076</v>
+      <c r="F22" s="80">
+        <v>144.3323292190903</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4398,8 +4685,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="38">
-        <v>0</v>
+      <c r="F23" s="78">
+        <v>88.73523092029185</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4418,8 +4705,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="38">
-        <v>0</v>
+      <c r="F24" s="80">
+        <v>143.2901716681866</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4438,8 +4725,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="38">
-        <v>0.1659259682065054</v>
+      <c r="F25" s="80">
+        <v>136.6083246091488</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4458,7 +4745,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="57">
+      <c r="F26" s="81">
         <v>3084.46527939775</v>
       </c>
     </row>
@@ -4478,7 +4765,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="58">
+      <c r="F27" s="82">
         <v>5218.548969676591</v>
       </c>
     </row>
@@ -4498,7 +4785,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="59">
+      <c r="F28" s="83">
         <v>7290.550607051456</v>
       </c>
     </row>
@@ -4518,8 +4805,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="60">
-        <v>157.9963648259174</v>
+      <c r="F29" s="84">
+        <v>582.134007671943</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4538,8 +4825,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="61">
-        <v>256.8775813585121</v>
+      <c r="F30" s="85">
+        <v>1375.553123106679</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4558,8 +4845,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="61">
-        <v>252.201973337168</v>
+      <c r="F31" s="54">
+        <v>3520.186422001009</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4578,8 +4865,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="38">
-        <v>7.004915824869674</v>
+      <c r="F32" s="79">
+        <v>173.7885881067872</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4598,8 +4885,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="38">
-        <v>19.88245120826813</v>
+      <c r="F33" s="86">
+        <v>593.5547460227471</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4618,8 +4905,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="38">
-        <v>26.52512966797964</v>
+      <c r="F34" s="87">
+        <v>503.0739806847629</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4638,8 +4925,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="38">
-        <v>0</v>
+      <c r="F35" s="75">
+        <v>209.2314853448774</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4658,8 +4945,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="38">
-        <v>0</v>
+      <c r="F36" s="84">
+        <v>579.5182342238497</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4678,8 +4965,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="38">
-        <v>1.00639298265476</v>
+      <c r="F37" s="87">
+        <v>492.521388025198</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4698,7 +4985,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="38">
+      <c r="F38" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4718,7 +5005,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4738,7 +5025,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="38">
+      <c r="F40" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4758,7 +5045,7 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="38">
+      <c r="F41" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4778,7 +5065,7 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="38">
+      <c r="F42" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4798,7 +5085,7 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F43" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4818,7 +5105,7 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4838,7 +5125,7 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="38">
+      <c r="F45" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4858,7 +5145,7 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="38">
+      <c r="F46" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4878,7 +5165,7 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F47" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4898,7 +5185,7 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4918,7 +5205,7 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="38">
+      <c r="F49" s="50">
         <v>0</v>
       </c>
     </row>
@@ -4938,7 +5225,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="36">
+      <c r="F50" s="48">
         <v>2033.809028558813</v>
       </c>
     </row>
@@ -4958,7 +5245,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="31">
+      <c r="F51" s="42">
         <v>3628.26835827906</v>
       </c>
     </row>
@@ -4978,7 +5265,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="62">
+      <c r="F52" s="88">
         <v>5019.446721344348</v>
       </c>
     </row>
@@ -4998,8 +5285,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="56">
-        <v>47.96078359189266</v>
+      <c r="F53" s="80">
+        <v>128.5209299243098</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -5018,8 +5305,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="56">
-        <v>66.20198877681104</v>
+      <c r="F54" s="89">
+        <v>373.2152226738353</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5038,8 +5325,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="56">
-        <v>47.96078359189266</v>
+      <c r="F55" s="90">
+        <v>1947.404849211568</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5058,8 +5345,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="38">
-        <v>2.044086645936808</v>
+      <c r="F56" s="91">
+        <v>43.08939876556691</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5078,8 +5365,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="38">
-        <v>4.104392192549324</v>
+      <c r="F57" s="78">
+        <v>74.26416509381531</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5098,8 +5385,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="38">
-        <v>5.048387286409375</v>
+      <c r="F58" s="91">
+        <v>54.23442527248671</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5118,8 +5405,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="38">
-        <v>0</v>
+      <c r="F59" s="91">
+        <v>51.51758776998382</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5138,8 +5425,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="38">
-        <v>0</v>
+      <c r="F60" s="78">
+        <v>93.97536146749252</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -5158,8 +5445,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="38">
-        <v>0.1028352577304621</v>
+      <c r="F61" s="91">
+        <v>67.75408785841486</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -5178,7 +5465,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="33">
+      <c r="F62" s="43">
         <v>3209.189600955568</v>
       </c>
     </row>
@@ -5198,7 +5485,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="63">
+      <c r="F63" s="92">
         <v>6452.649325876972</v>
       </c>
     </row>
@@ -5218,7 +5505,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="42">
+      <c r="F64" s="57">
         <v>9411.587846975366</v>
       </c>
     </row>
@@ -5238,8 +5525,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="64">
-        <v>116.2330709838142</v>
+      <c r="F65" s="93">
+        <v>332.5187650247582</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5258,8 +5545,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="61">
-        <v>225.6768717574853</v>
+      <c r="F66" s="94">
+        <v>1272.319450561094</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5278,8 +5565,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="65">
-        <v>191.1415546556391</v>
+      <c r="F67" s="47">
+        <v>3432.60832080301</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5298,8 +5585,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="38">
-        <v>3.707858343653531</v>
+      <c r="F68" s="78">
+        <v>76.79899375583491</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -5318,8 +5605,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="38">
-        <v>10.0352927215377</v>
+      <c r="F69" s="95">
+        <v>251.7820081772457</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5338,8 +5625,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="38">
-        <v>14.69020959038416</v>
+      <c r="F70" s="79">
+        <v>167.1821157144428</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -5358,8 +5645,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="38">
-        <v>0</v>
+      <c r="F71" s="78">
+        <v>88.79171050021246</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -5378,8 +5665,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="38">
-        <v>0</v>
+      <c r="F72" s="76">
+        <v>312.6598816286617</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -5398,8 +5685,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="38">
-        <v>0.5930210644548625</v>
+      <c r="F73" s="75">
+        <v>196.4518348469257</v>
       </c>
     </row>
   </sheetData>
@@ -5448,7 +5735,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="66">
+      <c r="F2" s="96">
         <v>803.1812751303619</v>
       </c>
     </row>
@@ -5468,7 +5755,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="97">
         <v>1873.499560122021</v>
       </c>
     </row>
@@ -5488,7 +5775,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="35">
         <v>2479.849226425816</v>
       </c>
     </row>
@@ -5508,8 +5795,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="67">
-        <v>68.92081261411315</v>
+      <c r="F5" s="14">
+        <v>209.1351481540951</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5528,8 +5815,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="68">
-        <v>147.9519858478812</v>
+      <c r="F6" s="98">
+        <v>707.5146876957986</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5548,8 +5835,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="69">
-        <v>114.82038821395</v>
+      <c r="F7" s="99">
+        <v>1039.132727636089</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5568,8 +5855,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8">
-        <v>3.015213234798099</v>
+      <c r="F8" s="20">
+        <v>72.22182267315955</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5588,8 +5875,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="8">
-        <v>8.971625035552561</v>
+      <c r="F9" s="100">
+        <v>284.1785960853406</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5608,8 +5895,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="6">
-        <v>12.81314494530556</v>
+      <c r="F10" s="101">
+        <v>162.2025650842136</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5628,8 +5915,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="8">
-        <v>0</v>
+      <c r="F11" s="102">
+        <v>85.30809430705875</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5648,8 +5935,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="8">
-        <v>0</v>
+      <c r="F12" s="103">
+        <v>302.3897650972152</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5668,8 +5955,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8">
-        <v>0.7389238865849204</v>
+      <c r="F13" s="104">
+        <v>187.4997506773731</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5688,7 +5975,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="100">
         <v>286.1479461511316</v>
       </c>
     </row>
@@ -5708,7 +5995,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="105">
         <v>879.5718154289259</v>
       </c>
     </row>
@@ -5728,7 +6015,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="72">
+      <c r="F16" s="106">
         <v>1251.282238116325</v>
       </c>
     </row>
@@ -5748,8 +6035,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="14">
-        <v>35.36254817001071</v>
+      <c r="F17" s="7">
+        <v>132.0844482284949</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5768,8 +6055,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="69">
-        <v>114.3937214037788</v>
+      <c r="F18" s="107">
+        <v>572.1466906127038</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5788,8 +6075,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="73">
-        <v>81.26212376984761</v>
+      <c r="F19" s="108">
+        <v>705.3848194274708</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -5808,8 +6095,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="8">
-        <v>0.4704435738192609</v>
+      <c r="F20" s="109">
+        <v>31.58162695801087</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -5828,8 +6115,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="8">
-        <v>3.063807613227472</v>
+      <c r="F21" s="14">
+        <v>213.0809433088728</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -5848,8 +6135,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="8">
-        <v>6.689821706106303</v>
+      <c r="F22" s="110">
+        <v>101.2635697430059</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5868,8 +6155,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="8">
-        <v>0</v>
+      <c r="F23" s="10">
+        <v>43.16053403909244</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -5888,8 +6175,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="8">
-        <v>0</v>
+      <c r="F24" s="111">
+        <v>238.8751099542148</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -5908,8 +6195,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="8">
-        <v>0.6365820223177816</v>
+      <c r="F25" s="112">
+        <v>123.9850955343727</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -5928,7 +6215,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>26.52956860275165</v>
       </c>
     </row>
@@ -5948,7 +6235,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="74">
+      <c r="F27" s="113">
         <v>447.2663866404827</v>
       </c>
     </row>
@@ -5968,7 +6255,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="75">
+      <c r="F28" s="114">
         <v>511.2861167504222</v>
       </c>
     </row>
@@ -5988,8 +6275,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="8">
-        <v>0</v>
+      <c r="F29" s="9">
+        <v>3.619028143245705</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6008,8 +6295,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="14">
-        <v>35.1876821059455</v>
+      <c r="F30" s="115">
+        <v>274.1454638673107</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6028,8 +6315,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="8">
-        <v>7.543543741909964</v>
+      <c r="F31" s="14">
+        <v>209.9954399747213</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6048,7 +6335,7 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6068,8 +6355,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="8">
-        <v>0.3194145032892469</v>
+      <c r="F33" s="18">
+        <v>57.55917790033037</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6088,8 +6375,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="8">
-        <v>1.353989690809433</v>
+      <c r="F34" s="9">
+        <v>1.365353281267226</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6108,7 +6395,7 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6128,8 +6415,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="8">
-        <v>0</v>
+      <c r="F36" s="102">
+        <v>80.07143737752703</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6148,8 +6435,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="8">
-        <v>0.2336632426461925</v>
+      <c r="F37" s="9">
+        <v>5.392442883357991</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6168,7 +6455,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="66">
+      <c r="F38" s="96">
         <v>803.1812751303619</v>
       </c>
     </row>
@@ -6188,7 +6475,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="97">
         <v>1873.499560122021</v>
       </c>
     </row>
@@ -6208,7 +6495,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="35">
         <v>2479.849226425816</v>
       </c>
     </row>
@@ -6228,8 +6515,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="76">
-        <v>52.82137228026796</v>
+      <c r="F41" s="116">
+        <v>141.7841065426883</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6248,8 +6535,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="69">
-        <v>110.9867958149954</v>
+      <c r="F42" s="117">
+        <v>500.6682095047611</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6268,8 +6555,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="77">
-        <v>87.28738592620482</v>
+      <c r="F43" s="118">
+        <v>834.8901557121877</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6288,8 +6575,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="8">
-        <v>1.825415749332406</v>
+      <c r="F44" s="109">
+        <v>32.9243005190282</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6308,8 +6595,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="8">
-        <v>4.96686534632999</v>
+      <c r="F45" s="110">
+        <v>102.5022070381353</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6328,8 +6615,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="8">
-        <v>8.592879439208822</v>
+      <c r="F46" s="20">
+        <v>68.80758320653729</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6348,8 +6635,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="8">
-        <v>0</v>
+      <c r="F47" s="109">
+        <v>36.50989849310458</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6368,8 +6655,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="8">
-        <v>0</v>
+      <c r="F48" s="7">
+        <v>134.2905711595562</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6388,8 +6675,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="8">
-        <v>0.5604719562918691</v>
+      <c r="F49" s="102">
+        <v>82.24745876379453</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6408,7 +6695,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="78">
+      <c r="F50" s="119">
         <v>203.3085743149552</v>
       </c>
     </row>
@@ -6428,7 +6715,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="79">
+      <c r="F51" s="98">
         <v>715.5014516919969</v>
       </c>
     </row>
@@ -6448,7 +6735,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="80">
+      <c r="F52" s="120">
         <v>908.2024087334084</v>
       </c>
     </row>
@@ -6468,8 +6755,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="7">
-        <v>27.06088525322274</v>
+      <c r="F53" s="20">
+        <v>77.17497435839286</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6488,8 +6775,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="67">
-        <v>76.85235353288284</v>
+      <c r="F54" s="121">
+        <v>332.7568242642446</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6508,8 +6795,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="81">
-        <v>61.52689889915959</v>
+      <c r="F55" s="115">
+        <v>277.3016052957108</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6528,8 +6815,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="8">
-        <v>0.6654984264945758</v>
+      <c r="F56" s="11">
+        <v>10.52065291011232</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6548,8 +6835,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="8">
-        <v>2.66406623806721</v>
+      <c r="F57" s="122">
+        <v>66.19990381458774</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6568,8 +6855,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="8">
-        <v>5.74134059351408</v>
+      <c r="F58" s="10">
+        <v>41.62982713791985</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6588,8 +6875,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="8">
-        <v>0</v>
+      <c r="F59" s="11">
+        <v>10.74941146605935</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6608,8 +6895,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="8">
-        <v>0</v>
+      <c r="F60" s="102">
+        <v>85.59946363447793</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6628,8 +6915,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="8">
-        <v>0.4970439582377673</v>
+      <c r="F61" s="10">
+        <v>46.50818173791374</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6648,7 +6935,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F62" s="9">
         <v>0.1834627105676357</v>
       </c>
     </row>
@@ -6668,7 +6955,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="78">
+      <c r="F63" s="119">
         <v>198.6769964578388</v>
       </c>
     </row>
@@ -6688,7 +6975,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="73">
+      <c r="F64" s="102">
         <v>79.96340726237918</v>
       </c>
     </row>
@@ -6708,8 +6995,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="8">
-        <v>0.1834611825710685</v>
+      <c r="F65" s="9">
+        <v>0.1834626616105195</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6728,8 +7015,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="6">
-        <v>13.84653115016949</v>
+      <c r="F66" s="102">
+        <v>81.29373680669678</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6748,8 +7035,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="8">
-        <v>2.320999470766093</v>
+      <c r="F67" s="11">
+        <v>13.30665948623112</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6768,8 +7055,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="8">
-        <v>0.1698723992805488</v>
+      <c r="F68" s="9">
+        <v>0.1830272760493846</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -6788,8 +7075,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="8">
-        <v>0.5240821687332275</v>
+      <c r="F69" s="9">
+        <v>0.5372370455020633</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -6808,8 +7095,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="8">
-        <v>1.974328413627587</v>
+      <c r="F70" s="9">
+        <v>2.257844340878407</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -6828,8 +7115,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="8">
-        <v>0</v>
+      <c r="F71" s="9">
+        <v>0.1414736192097876</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -6848,8 +7135,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="8">
-        <v>0</v>
+      <c r="F72" s="9">
+        <v>0.4956833886624665</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -6868,8 +7155,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="8">
-        <v>0.2617295567876485</v>
+      <c r="F73" s="9">
+        <v>1.973204017953146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated V2G scenarios and plots
</commit_message>
<xml_diff>
--- a/results/Manuscript/material_use.xlsx
+++ b/results/Manuscript/material_use.xlsx
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="122">
+  <fills count="130">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,7 +126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5C8C7"/>
+        <fgColor rgb="FFF5C8C8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,36 +162,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF3EAEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF3ECEC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF4E1E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5CBCB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5BEBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EBEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF3EFEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5CBCB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5BEBE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DCDC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF5CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -210,18 +234,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3EBEB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF5C4C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF3E8E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF3E9E9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -246,31 +270,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF97070"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6868"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97171"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF96F6F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA6868"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97171"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97070"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4949"/>
+        <fgColor rgb="FFF97272"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB4A4A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,19 +312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA6969"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA5F5F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97272"/>
+        <fgColor rgb="FFFA5E5E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,13 +336,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF96E6E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA6262"/>
+        <fgColor rgb="FFF96D6D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,30 +420,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF99CB99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1CFA1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCDCBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94C994"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9ACB9A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF98CA98"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA0CEA0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBCDCBC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF97CA97"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -456,6 +486,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF028102"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF068306"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -510,13 +546,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF148A14"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF319831"/>
+        <fgColor rgb="FF178B17"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF339933"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0A850A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,126 +600,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4E8D4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F1E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9ECE9E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF69B369"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF349A34"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCECDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8E2C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5F0E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEBDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8EAD8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDECDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFEDDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DB66D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EEE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBDCBB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAF2EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4AA44A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4F0E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7E1C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EEE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE3EFE3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3E7D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9F2E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7F1E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2E8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ECE9E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF69B369"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF349A34"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDECDD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC9E2C8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDCECDC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDFEDDF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6DB66D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1EEE1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBDCBB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEAF2EA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4AA44A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFE2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCBE4CB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5F0E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF7A3A3"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -690,151 +756,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF88989"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D7D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E8E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DEDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D5D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79B9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97777"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B8B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E5E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C5C5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5BFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DADA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79D9D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF6ABAB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF88B8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D5D5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4E1E1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E8E8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DEDE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79B9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97777"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6B8B8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6ACAC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EDED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E7E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E5E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C5C5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5BFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D6D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E3E3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C0C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79F9F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DDDD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF79898"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4D0D0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EAEA"/>
+        <fgColor rgb="FFF4CFCF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -890,10 +938,10 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -907,8 +955,8 @@
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -925,60 +973,60 @@
     <xf numFmtId="0" fontId="2" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="75" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="75" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="78" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="79" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="80" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="81" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="82" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="81" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="82" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="83" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="84" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="85" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="90" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="91" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="91" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="92" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="93" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="94" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="95" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="96" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="97" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="98" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="96" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="97" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="98" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="99" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="100" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="102" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="103" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="104" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="105" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="105" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="106" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="109" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="110" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="111" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -986,12 +1034,20 @@
     <xf numFmtId="0" fontId="2" fillId="113" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="114" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="115" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="116" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="116" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="117" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="118" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="119" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="120" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="121" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="122" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="123" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="124" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="125" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="126" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="127" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="128" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="129" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,7 +1442,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="6">
-        <v>37490.49492452692</v>
+        <v>37498.43080197114</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1406,7 +1462,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="7">
-        <v>37887.56661130874</v>
+        <v>37902.63267189218</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1426,7 +1482,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="8">
-        <v>38212.80964096187</v>
+        <v>38231.43766327716</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1446,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="9">
-        <v>37385.76194420527</v>
+        <v>37410.71985159518</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1466,7 +1522,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="10">
-        <v>37545.99352427768</v>
+        <v>37621.04873812848</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1486,7 +1542,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="11">
-        <v>37453.02879417115</v>
+        <v>37537.15574481436</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1506,7 +1562,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="9">
-        <v>37395.54083966072</v>
+        <v>37395.5408395745</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1525,8 +1581,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="10">
-        <v>37559.4511818316</v>
+      <c r="F12" s="12">
+        <v>37559.45118173854</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1546,7 +1602,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="6">
-        <v>37472.21420633512</v>
+        <v>37472.21420624205</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1565,7 +1621,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="13">
         <v>38027.6536108783</v>
       </c>
     </row>
@@ -1585,7 +1641,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="14">
         <v>38862.37038121407</v>
       </c>
     </row>
@@ -1605,7 +1661,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="15">
         <v>39409.03516301885</v>
       </c>
     </row>
@@ -1626,7 +1682,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="6">
-        <v>37483.88802480543</v>
+        <v>37489.88472757782</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1646,7 +1702,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="7">
-        <v>37872.04289509112</v>
+        <v>37887.37253452981</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1665,8 +1721,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="14">
-        <v>38189.8711056198</v>
+      <c r="F19" s="16">
+        <v>38200.3933659232</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1686,7 +1742,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="9">
-        <v>37379.58649703812</v>
+        <v>37402.82638715756</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1705,8 +1761,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="10">
-        <v>37537.94697893425</v>
+      <c r="F21" s="17">
+        <v>37610.51451471172</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1726,7 +1782,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="11">
-        <v>37448.19082480113</v>
+        <v>37527.02778757971</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1746,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="9">
-        <v>37389.50869071848</v>
+        <v>37389.50869061065</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1765,8 +1821,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="10">
-        <v>37552.30761756487</v>
+      <c r="F24" s="12">
+        <v>37552.30761752666</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1785,8 +1841,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="6">
-        <v>37463.17788648279</v>
+      <c r="F25" s="18">
+        <v>37463.17788638971</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1805,7 +1861,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="19">
         <v>38820.09493073855</v>
       </c>
     </row>
@@ -1825,7 +1881,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="20">
         <v>40176.08684177568</v>
       </c>
     </row>
@@ -1845,7 +1901,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="21">
         <v>41241.89777610592</v>
       </c>
     </row>
@@ -1865,8 +1921,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="18">
-        <v>37603.96999706588</v>
+      <c r="F29" s="17">
+        <v>37612.86830548158</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1885,8 +1941,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="14">
-        <v>38186.62819753488</v>
+      <c r="F30" s="16">
+        <v>38209.37177112736</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1905,8 +1961,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="19">
-        <v>39170.48945010785</v>
+      <c r="F31" s="22">
+        <v>39179.1577698071</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1925,8 +1981,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="9">
-        <v>37411.42027899526</v>
+      <c r="F32" s="18">
+        <v>37448.38755813866</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1945,8 +2001,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="20">
-        <v>37648.1056894984</v>
+      <c r="F33" s="23">
+        <v>37740.03366767087</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1965,8 +2021,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="10">
-        <v>37564.1745709563</v>
+      <c r="F34" s="24">
+        <v>37686.53228787622</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1985,8 +2041,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="11">
-        <v>37427.75303016329</v>
+      <c r="F35" s="18">
+        <v>37427.7530300599</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2005,8 +2061,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="20">
-        <v>37658.53375115538</v>
+      <c r="F36" s="24">
+        <v>37658.53375119837</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2025,8 +2081,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="10">
-        <v>37561.84975887099</v>
+      <c r="F37" s="12">
+        <v>37561.84975889421</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2045,7 +2101,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="21">
+      <c r="F38" s="25">
         <v>43146.87751981514</v>
       </c>
     </row>
@@ -2065,7 +2121,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="26">
         <v>44101.76903663111</v>
       </c>
     </row>
@@ -2085,7 +2141,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="27">
         <v>44694.68505036762</v>
       </c>
     </row>
@@ -2105,8 +2161,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="24">
-        <v>42541.9678382339</v>
+      <c r="F41" s="28">
+        <v>42520.59871654321</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2125,8 +2181,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="25">
-        <v>42821.7152006235</v>
+      <c r="F42" s="29">
+        <v>42840.58392931787</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2145,8 +2201,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="21">
-        <v>43155.50989436005</v>
+      <c r="F43" s="25">
+        <v>43175.26330096238</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2165,8 +2221,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="26">
-        <v>42460.78688361657</v>
+      <c r="F44" s="30">
+        <v>42470.88661173557</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2185,8 +2241,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="27">
-        <v>42511.77039385081</v>
+      <c r="F45" s="31">
+        <v>42565.16501139421</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2205,8 +2261,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="26">
-        <v>42486.90840482202</v>
+      <c r="F46" s="28">
+        <v>42509.63678944725</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2225,8 +2281,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="26">
-        <v>42463.42532364777</v>
+      <c r="F47" s="32">
+        <v>42463.42532364507</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2245,8 +2301,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="24">
-        <v>42535.51332075584</v>
+      <c r="F48" s="28">
+        <v>42535.51332053153</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2265,8 +2321,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="26">
-        <v>42496.8518929108</v>
+      <c r="F49" s="30">
+        <v>42496.8518928113</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2285,7 +2341,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="21">
+      <c r="F50" s="25">
         <v>43174.29827220868</v>
       </c>
     </row>
@@ -2305,7 +2361,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="28">
+      <c r="F51" s="33">
         <v>44042.88994517744</v>
       </c>
     </row>
@@ -2325,7 +2381,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="29">
+      <c r="F52" s="34">
         <v>44632.76660394678</v>
       </c>
     </row>
@@ -2345,8 +2401,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="27">
-        <v>42529.41815279475</v>
+      <c r="F53" s="28">
+        <v>42508.61373339163</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2365,8 +2421,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="30">
-        <v>42792.54578025143</v>
+      <c r="F54" s="29">
+        <v>42810.90772176443</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2385,8 +2441,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="31">
-        <v>43207.54276501382</v>
+      <c r="F55" s="35">
+        <v>43223.79136664226</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2405,8 +2461,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="32">
-        <v>42456.26732785177</v>
+      <c r="F56" s="30">
+        <v>42464.8913964779</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2425,8 +2481,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="27">
-        <v>42505.64278778723</v>
+      <c r="F57" s="31">
+        <v>42552.94645746489</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2445,8 +2501,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="26">
-        <v>42481.97457043862</v>
+      <c r="F58" s="28">
+        <v>42501.77369760885</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2466,7 +2522,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="32">
-        <v>42458.78580147695</v>
+        <v>42458.78580141172</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2485,8 +2541,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="27">
-        <v>42525.5570406761</v>
+      <c r="F60" s="28">
+        <v>42525.5570404518</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2505,8 +2561,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="26">
-        <v>42489.3349762876</v>
+      <c r="F61" s="30">
+        <v>42489.33497618809</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2525,7 +2581,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="33">
+      <c r="F62" s="36">
         <v>43964.38010005821</v>
       </c>
     </row>
@@ -2545,7 +2601,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="34">
+      <c r="F63" s="37">
         <v>45673.59602566905</v>
       </c>
     </row>
@@ -2565,7 +2621,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="35">
+      <c r="F64" s="38">
         <v>47012.52701914091</v>
       </c>
     </row>
@@ -2585,8 +2641,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="36">
-        <v>42585.87510575628</v>
+      <c r="F65" s="31">
+        <v>42566.92361934109</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2605,8 +2661,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="37">
-        <v>43080.9108578156</v>
+      <c r="F66" s="25">
+        <v>43145.31036802677</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2625,8 +2681,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="28">
-        <v>44073.93921209701</v>
+      <c r="F67" s="26">
+        <v>44138.37101440705</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2645,8 +2701,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="26">
-        <v>42470.65558151645</v>
+      <c r="F68" s="30">
+        <v>42485.48141090687</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2665,8 +2721,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="24">
-        <v>42548.68478832724</v>
+      <c r="F69" s="39">
+        <v>42621.29943980042</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2685,8 +2741,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="27">
-        <v>42511.98215560726</v>
+      <c r="F70" s="31">
+        <v>42545.97011032965</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2705,8 +2761,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="26">
-        <v>42476.01538714891</v>
+      <c r="F71" s="30">
+        <v>42476.0153870825</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2725,8 +2781,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="36">
-        <v>42576.14125782856</v>
+      <c r="F72" s="31">
+        <v>42576.14125754007</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2745,8 +2801,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="27">
-        <v>42524.91536581161</v>
+      <c r="F73" s="28">
+        <v>42524.91536559458</v>
       </c>
     </row>
   </sheetData>
@@ -2795,7 +2851,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="40">
         <v>7526.317007325268</v>
       </c>
     </row>
@@ -2815,7 +2871,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="41">
         <v>7641.74377550096</v>
       </c>
     </row>
@@ -2835,7 +2891,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="42">
         <v>7655.177428068251</v>
       </c>
     </row>
@@ -2855,8 +2911,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="38">
-        <v>7484.587833051628</v>
+      <c r="F5" s="40">
+        <v>7485.283081260031</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2875,8 +2931,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="41">
-        <v>7585.895685811509</v>
+      <c r="F6" s="43">
+        <v>7587.658791039436</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2895,8 +2951,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="41">
-        <v>7592.270696098678</v>
+      <c r="F7" s="43">
+        <v>7594.339770659917</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2915,8 +2971,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="42">
-        <v>7452.407487892349</v>
+      <c r="F8" s="44">
+        <v>7460.618440913315</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2935,8 +2991,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="38">
-        <v>7504.132681232119</v>
+      <c r="F9" s="40">
+        <v>7525.584462536903</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2955,8 +3011,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="38">
-        <v>7475.121380337516</v>
+      <c r="F10" s="40">
+        <v>7498.378400995356</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2975,8 +3031,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="42">
-        <v>7455.714864070796</v>
+      <c r="F11" s="44">
+        <v>7455.714864042428</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2995,8 +3051,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="38">
-        <v>7508.886192690064</v>
+      <c r="F12" s="40">
+        <v>7508.886192658765</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3015,8 +3071,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="38">
-        <v>7481.233153766711</v>
+      <c r="F13" s="40">
+        <v>7481.233153735411</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3035,7 +3091,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="45">
         <v>7024.441944697281</v>
       </c>
     </row>
@@ -3055,7 +3111,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="46">
         <v>6783.149043639318</v>
       </c>
     </row>
@@ -3075,7 +3131,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="47">
         <v>6608.194684521932</v>
       </c>
     </row>
@@ -3095,8 +3151,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="46">
-        <v>7414.14403284752</v>
+      <c r="F17" s="48">
+        <v>7410.456130585966</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3115,8 +3171,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="42">
-        <v>7466.051404946031</v>
+      <c r="F18" s="44">
+        <v>7465.797623001579</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3135,8 +3191,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="47">
-        <v>7281.461323232128</v>
+      <c r="F19" s="49">
+        <v>7291.101151940789</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3155,8 +3211,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="46">
-        <v>7417.942739344348</v>
+      <c r="F20" s="48">
+        <v>7416.477715263414</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3175,8 +3231,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="42">
-        <v>7441.081573799078</v>
+      <c r="F21" s="44">
+        <v>7459.067986028058</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3195,8 +3251,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="46">
-        <v>7419.020354366328</v>
+      <c r="F22" s="48">
+        <v>7420.578682158948</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3215,8 +3271,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="46">
-        <v>7419.599452745066</v>
+      <c r="F23" s="48">
+        <v>7419.599452738314</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3235,8 +3291,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="42">
-        <v>7452.515101813799</v>
+      <c r="F24" s="44">
+        <v>7452.515101727635</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3255,8 +3311,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="46">
-        <v>7426.75481847604</v>
+      <c r="F25" s="48">
+        <v>7426.754818444741</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3275,7 +3331,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="50">
         <v>5972.38224728867</v>
       </c>
     </row>
@@ -3295,7 +3351,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="49">
+      <c r="F27" s="51">
         <v>5037.127154289265</v>
       </c>
     </row>
@@ -3315,7 +3371,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="52">
         <v>4035.335950068962</v>
       </c>
     </row>
@@ -3335,8 +3391,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="51">
-        <v>7165.596640501826</v>
+      <c r="F29" s="53">
+        <v>7153.079303942879</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3355,8 +3411,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="52">
-        <v>6853.464875756896</v>
+      <c r="F30" s="54">
+        <v>6839.923419658385</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3375,8 +3431,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="53">
-        <v>5805.453599291333</v>
+      <c r="F31" s="55">
+        <v>5813.728243882939</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3395,8 +3451,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="54">
-        <v>7354.527330429212</v>
+      <c r="F32" s="56">
+        <v>7317.560051285805</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3415,8 +3471,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="51">
-        <v>7175.401097826402</v>
+      <c r="F33" s="53">
+        <v>7142.294514734924</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3435,8 +3491,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="55">
-        <v>7203.138391749419</v>
+      <c r="F34" s="57">
+        <v>7093.57160599095</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3455,8 +3511,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="54">
-        <v>7338.194579261172</v>
+      <c r="F35" s="58">
+        <v>7338.19457936457</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3475,8 +3531,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="51">
-        <v>7187.485295646615</v>
+      <c r="F36" s="59">
+        <v>7187.485295435928</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3495,8 +3551,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="55">
-        <v>7209.490293436837</v>
+      <c r="F37" s="60">
+        <v>7209.490293347926</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3515,7 +3571,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="56">
+      <c r="F38" s="61">
         <v>12788.24710269182</v>
       </c>
     </row>
@@ -3535,7 +3591,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="57">
+      <c r="F39" s="62">
         <v>12903.67387086751</v>
       </c>
     </row>
@@ -3555,7 +3611,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="57">
+      <c r="F40" s="62">
         <v>12917.1075234348</v>
       </c>
     </row>
@@ -3575,8 +3631,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="58">
-        <v>12731.7596156854</v>
+      <c r="F41" s="63">
+        <v>12723.94673328884</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3595,8 +3651,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="56">
-        <v>12810.89635625786</v>
+      <c r="F42" s="61">
+        <v>12812.05655727977</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3615,8 +3671,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="56">
-        <v>12811.32360872874</v>
+      <c r="F43" s="64">
+        <v>12813.56055257101</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3635,8 +3691,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="59">
-        <v>12704.08076427906</v>
+      <c r="F44" s="65">
+        <v>12707.70495710543</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3655,8 +3711,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="58">
-        <v>12722.67516056393</v>
+      <c r="F45" s="63">
+        <v>12740.41452118682</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3675,8 +3731,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="58">
-        <v>12713.84252576112</v>
+      <c r="F46" s="63">
+        <v>12721.77322022874</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3695,8 +3751,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="59">
-        <v>12705.02792222194</v>
+      <c r="F47" s="65">
+        <v>12705.02792222202</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3715,8 +3771,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="58">
-        <v>12730.72059778032</v>
+      <c r="F48" s="63">
+        <v>12730.72059770548</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3735,8 +3791,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="58">
-        <v>12717.33891322959</v>
+      <c r="F49" s="63">
+        <v>12717.33891319589</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3755,7 +3811,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="60">
+      <c r="F50" s="66">
         <v>12160.95364948288</v>
       </c>
     </row>
@@ -3775,7 +3831,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="61">
+      <c r="F51" s="67">
         <v>11804.55485389116</v>
       </c>
     </row>
@@ -3795,7 +3851,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="62">
+      <c r="F52" s="68">
         <v>11407.37915216324</v>
       </c>
     </row>
@@ -3815,8 +3871,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="59">
-        <v>12679.70016894025</v>
+      <c r="F53" s="65">
+        <v>12664.7364139125</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3835,8 +3891,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="59">
-        <v>12672.15439138942</v>
+      <c r="F54" s="65">
+        <v>12666.03761672571</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3855,8 +3911,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="63">
-        <v>12201.70218765849</v>
+      <c r="F55" s="69">
+        <v>12210.66838903153</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3875,8 +3931,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="59">
-        <v>12686.19667243494</v>
+      <c r="F56" s="65">
+        <v>12682.47762842492</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3895,8 +3951,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="59">
-        <v>12692.50046340397</v>
+      <c r="F57" s="65">
+        <v>12688.55622056666</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3915,8 +3971,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="59">
-        <v>12691.5986040759</v>
+      <c r="F58" s="65">
+        <v>12686.97816980611</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3935,8 +3991,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="59">
-        <v>12683.90695736571</v>
+      <c r="F59" s="65">
+        <v>12683.90695742833</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3955,8 +4011,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="59">
-        <v>12691.98577033498</v>
+      <c r="F60" s="65">
+        <v>12691.98577026014</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3975,8 +4031,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="59">
-        <v>12689.11655282692</v>
+      <c r="F61" s="65">
+        <v>12689.11655279322</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3995,7 +4051,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="64">
+      <c r="F62" s="70">
         <v>11167.74671002897</v>
       </c>
     </row>
@@ -4015,7 +4071,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="65">
+      <c r="F63" s="71">
         <v>9657.024318165388</v>
       </c>
     </row>
@@ -4035,7 +4091,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="66">
+      <c r="F64" s="72">
         <v>8199.379735498071</v>
       </c>
     </row>
@@ -4055,8 +4111,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="67">
-        <v>12546.25170428193</v>
+      <c r="F65" s="73">
+        <v>12565.20179025661</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4075,8 +4131,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="68">
-        <v>12132.32622636768</v>
+      <c r="F66" s="74">
+        <v>12032.90436236553</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4095,8 +4151,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="69">
-        <v>11071.31079476583</v>
+      <c r="F67" s="75">
+        <v>10995.81925105556</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4115,8 +4171,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="59">
-        <v>12661.47079313621</v>
+      <c r="F68" s="65">
+        <v>12646.64448946467</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4135,8 +4191,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="70">
-        <v>12583.79579609485</v>
+      <c r="F69" s="76">
+        <v>12513.81629815426</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4155,8 +4211,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="71">
-        <v>12622.21903611022</v>
+      <c r="F70" s="77">
+        <v>12588.2210465781</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4175,8 +4231,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="59">
-        <v>12656.0694338469</v>
+      <c r="F71" s="65">
+        <v>12656.06943391686</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4195,8 +4251,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="67">
-        <v>12556.2977729367</v>
+      <c r="F72" s="73">
+        <v>12556.29777322873</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4215,8 +4271,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="71">
-        <v>12609.00118558295</v>
+      <c r="F73" s="78">
+        <v>12609.0011858149</v>
       </c>
     </row>
   </sheetData>
@@ -4265,7 +4321,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="50">
+      <c r="F2" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4285,7 +4341,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4305,7 +4361,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4325,7 +4381,7 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4345,7 +4401,7 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4365,7 +4421,7 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4385,7 +4441,7 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4405,7 +4461,7 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="50">
+      <c r="F9" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4425,7 +4481,7 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="50">
+      <c r="F10" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4445,7 +4501,7 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4465,7 +4521,7 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4485,7 +4541,7 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="52">
         <v>0</v>
       </c>
     </row>
@@ -4505,7 +4561,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="79">
         <v>1650.829858861342</v>
       </c>
     </row>
@@ -4525,7 +4581,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="73">
+      <c r="F15" s="80">
         <v>2881.854852240659</v>
       </c>
     </row>
@@ -4545,7 +4601,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="74">
+      <c r="F16" s="81">
         <v>3533.499652148049</v>
       </c>
     </row>
@@ -4565,8 +4621,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="75">
-        <v>183.827075772615</v>
+      <c r="F17" s="82">
+        <v>195.6104432047388</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4585,8 +4641,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="76">
-        <v>330.513716496191</v>
+      <c r="F18" s="83">
+        <v>336.9535906915762</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4605,8 +4661,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="77">
-        <v>976.3257276115362</v>
+      <c r="F19" s="84">
+        <v>949.6895523472003</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4625,8 +4681,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="78">
-        <v>84.24558607264686</v>
+      <c r="F20" s="85">
+        <v>108.8522090549048</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4645,8 +4701,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="79">
-        <v>161.7408486386202</v>
+      <c r="F21" s="86">
+        <v>169.9460619159358</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4665,8 +4721,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="80">
-        <v>144.3323292190903</v>
+      <c r="F22" s="82">
+        <v>203.4457937514989</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4685,8 +4741,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="78">
-        <v>88.73523092029185</v>
+      <c r="F23" s="85">
+        <v>88.73523084425588</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4705,8 +4761,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="80">
-        <v>143.2901716681866</v>
+      <c r="F24" s="87">
+        <v>143.290171861868</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4725,7 +4781,7 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="80">
+      <c r="F25" s="87">
         <v>136.6083246091488</v>
       </c>
     </row>
@@ -4745,7 +4801,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="81">
+      <c r="F26" s="88">
         <v>3084.46527939775</v>
       </c>
     </row>
@@ -4765,7 +4821,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="82">
+      <c r="F27" s="89">
         <v>5218.548969676591</v>
       </c>
     </row>
@@ -4785,7 +4841,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="83">
+      <c r="F28" s="90">
         <v>7290.550607051456</v>
       </c>
     </row>
@@ -4805,8 +4861,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="84">
-        <v>582.134007671943</v>
+      <c r="F29" s="91">
+        <v>606.084637217702</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4825,8 +4881,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="85">
-        <v>1375.553123106679</v>
+      <c r="F30" s="92">
+        <v>1405.663904701903</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4845,8 +4901,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="54">
-        <v>3520.186422001009</v>
+      <c r="F31" s="58">
+        <v>3506.802908930157</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4865,8 +4921,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="79">
-        <v>173.7885881067872</v>
+      <c r="F32" s="93">
+        <v>254.0593554738107</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4885,8 +4941,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="86">
-        <v>593.5547460227471</v>
+      <c r="F33" s="94">
+        <v>693.7358982401573</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4905,8 +4961,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="87">
-        <v>503.0739806847629</v>
+      <c r="F34" s="95">
+        <v>744.1541077626994</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4925,8 +4981,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="75">
-        <v>209.2314853448774</v>
+      <c r="F35" s="82">
+        <v>209.2314851255441</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4945,8 +5001,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="84">
-        <v>579.5182342238497</v>
+      <c r="F36" s="96">
+        <v>579.5182345907845</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4965,8 +5021,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="87">
-        <v>492.521388025198</v>
+      <c r="F37" s="97">
+        <v>492.5213881821418</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4985,7 +5041,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="50">
+      <c r="F38" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5005,7 +5061,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5025,7 +5081,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="50">
+      <c r="F40" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5045,7 +5101,7 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="50">
+      <c r="F41" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5065,7 +5121,7 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="50">
+      <c r="F42" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5085,7 +5141,7 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="50">
+      <c r="F43" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5105,7 +5161,7 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="50">
+      <c r="F44" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5125,7 +5181,7 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="50">
+      <c r="F45" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5145,7 +5201,7 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="50">
+      <c r="F46" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5165,7 +5221,7 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="50">
+      <c r="F47" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5185,7 +5241,7 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="50">
+      <c r="F48" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5205,7 +5261,7 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="50">
+      <c r="F49" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5225,7 +5281,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="48">
+      <c r="F50" s="50">
         <v>2033.809028558813</v>
       </c>
     </row>
@@ -5245,7 +5301,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="42">
+      <c r="F51" s="44">
         <v>3628.26835827906</v>
       </c>
     </row>
@@ -5265,7 +5321,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="88">
+      <c r="F52" s="98">
         <v>5019.446721344348</v>
       </c>
     </row>
@@ -5285,8 +5341,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="80">
-        <v>128.5209299243098</v>
+      <c r="F53" s="86">
+        <v>149.1270711280139</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -5305,8 +5361,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="89">
-        <v>373.2152226738353</v>
+      <c r="F54" s="99">
+        <v>395.269390458085</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5325,8 +5381,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="90">
-        <v>1947.404849211568</v>
+      <c r="F55" s="100">
+        <v>1922.706280258855</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5345,8 +5401,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="91">
-        <v>43.08939876556691</v>
+      <c r="F56" s="101">
+        <v>61.19266001313503</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5365,8 +5421,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="78">
-        <v>74.26416509381531</v>
+      <c r="F57" s="87">
+        <v>128.2441842873131</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5385,8 +5441,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="91">
-        <v>54.23442527248671</v>
+      <c r="F58" s="85">
+        <v>85.19809325586476</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5405,8 +5461,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="91">
-        <v>51.51758776998382</v>
+      <c r="F59" s="101">
+        <v>51.51758754533567</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5425,7 +5481,7 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="78">
+      <c r="F60" s="85">
         <v>93.97536146749252</v>
       </c>
     </row>
@@ -5445,7 +5501,7 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="91">
+      <c r="F61" s="101">
         <v>67.75408785841486</v>
       </c>
     </row>
@@ -5465,7 +5521,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="43">
+      <c r="F62" s="45">
         <v>3209.189600955568</v>
       </c>
     </row>
@@ -5485,7 +5541,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="92">
+      <c r="F63" s="102">
         <v>6452.649325876972</v>
       </c>
     </row>
@@ -5505,7 +5561,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="57">
+      <c r="F64" s="62">
         <v>9411.587846975366</v>
       </c>
     </row>
@@ -5525,8 +5581,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="93">
-        <v>332.5187650247582</v>
+      <c r="F65" s="103">
+        <v>289.4256474956678</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5545,8 +5601,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="94">
-        <v>1272.319450561094</v>
+      <c r="F66" s="104">
+        <v>1464.817806165867</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5565,8 +5621,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="47">
-        <v>3432.60832080301</v>
+      <c r="F67" s="48">
+        <v>3583.372124797327</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5585,8 +5641,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="78">
-        <v>76.79899375583491</v>
+      <c r="F68" s="85">
+        <v>110.0044816763576</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -5605,8 +5661,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="95">
-        <v>251.7820081772457</v>
+      <c r="F69" s="105">
+        <v>407.8904046906079</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5625,8 +5681,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="79">
-        <v>167.1821157144428</v>
+      <c r="F70" s="93">
+        <v>242.8329589295964</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -5645,8 +5701,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="78">
-        <v>88.79171050021246</v>
+      <c r="F71" s="85">
+        <v>88.79171035304222</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -5665,8 +5721,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="76">
-        <v>312.6598816286617</v>
+      <c r="F72" s="106">
+        <v>312.6598809927535</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -5685,8 +5741,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="75">
-        <v>196.4518348469257</v>
+      <c r="F73" s="82">
+        <v>196.4518343454459</v>
       </c>
     </row>
   </sheetData>
@@ -5735,7 +5791,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="96">
+      <c r="F2" s="107">
         <v>803.1812751303619</v>
       </c>
     </row>
@@ -5755,7 +5811,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="97">
+      <c r="F3" s="108">
         <v>1873.499560122021</v>
       </c>
     </row>
@@ -5775,7 +5831,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="38">
         <v>2479.849226425816</v>
       </c>
     </row>
@@ -5795,8 +5851,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14">
-        <v>209.1351481540951</v>
+      <c r="F5" s="8">
+        <v>217.7662738067129</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5815,8 +5871,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="98">
-        <v>707.5146876957986</v>
+      <c r="F6" s="20">
+        <v>724.343853507159</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5835,8 +5891,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="99">
-        <v>1039.132727636089</v>
+      <c r="F7" s="109">
+        <v>1059.829824512622</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5855,8 +5911,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="20">
-        <v>72.22182267315955</v>
+      <c r="F8" s="110">
+        <v>105.3906830840426</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5875,8 +5931,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="100">
-        <v>284.1785960853406</v>
+      <c r="F9" s="14">
+        <v>380.6855912409278</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5895,8 +5951,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101">
-        <v>162.2025650842136</v>
+      <c r="F10" s="111">
+        <v>269.5865363852637</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5915,8 +5971,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="102">
-        <v>85.30809430705875</v>
+      <c r="F11" s="112">
+        <v>85.30809419247382</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5935,8 +5991,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="103">
-        <v>302.3897650972152</v>
+      <c r="F12" s="113">
+        <v>302.3897649728449</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5955,8 +6011,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="104">
-        <v>187.4997506773731</v>
+      <c r="F13" s="114">
+        <v>187.4997505530028</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5975,7 +6031,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="100">
+      <c r="F14" s="115">
         <v>286.1479461511316</v>
       </c>
     </row>
@@ -5995,7 +6051,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="105">
+      <c r="F15" s="116">
         <v>879.5718154289259</v>
       </c>
     </row>
@@ -6015,7 +6071,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="106">
+      <c r="F16" s="117">
         <v>1251.282238116325</v>
       </c>
     </row>
@@ -6036,7 +6092,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="7">
-        <v>132.0844482284949</v>
+        <v>134.3932487393278</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6055,8 +6111,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="107">
-        <v>572.1466906127038</v>
+      <c r="F18" s="118">
+        <v>587.222548106937</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6075,8 +6131,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="108">
-        <v>705.3848194274708</v>
+      <c r="F19" s="20">
+        <v>725.5469084395307</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6095,8 +6151,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="109">
-        <v>31.58162695801087</v>
+      <c r="F20" s="17">
+        <v>53.3564929965241</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6115,8 +6171,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="14">
-        <v>213.0809433088728</v>
+      <c r="F21" s="113">
+        <v>303.6348913153278</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -6135,8 +6191,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="110">
-        <v>101.2635697430059</v>
+      <c r="F22" s="119">
+        <v>181.6588603142008</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6155,8 +6211,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="10">
-        <v>43.16053403909244</v>
+      <c r="F23" s="12">
+        <v>43.16053392450752</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6175,8 +6231,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="111">
-        <v>238.8751099542148</v>
+      <c r="F24" s="120">
+        <v>238.8751098298445</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6195,8 +6251,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="112">
-        <v>123.9850955343727</v>
+      <c r="F25" s="121">
+        <v>123.9850954100024</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6235,7 +6291,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="113">
+      <c r="F27" s="122">
         <v>447.2663866404827</v>
       </c>
     </row>
@@ -6255,7 +6311,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="114">
+      <c r="F28" s="123">
         <v>511.2861167504222</v>
       </c>
     </row>
@@ -6276,7 +6332,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="9">
-        <v>3.619028143245705</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6296,7 +6352,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="115">
-        <v>274.1454638673107</v>
+        <v>283.3475813612906</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6315,8 +6371,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="14">
-        <v>209.9954399747213</v>
+      <c r="F31" s="124">
+        <v>226.9384042655693</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6355,8 +6411,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="18">
-        <v>57.55917790033037</v>
+      <c r="F33" s="121">
+        <v>116.3805729813275</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6375,8 +6431,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="9">
-        <v>1.365353281267226</v>
+      <c r="F34" s="18">
+        <v>14.15628444271354</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6415,8 +6471,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="102">
-        <v>80.07143737752703</v>
+      <c r="F36" s="112">
+        <v>80.07143720982413</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6436,7 +6492,7 @@
         <v>15</v>
       </c>
       <c r="F37" s="9">
-        <v>5.392442883357991</v>
+        <v>5.392442817685369</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6455,7 +6511,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="96">
+      <c r="F38" s="107">
         <v>803.1812751303619</v>
       </c>
     </row>
@@ -6475,7 +6531,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="97">
+      <c r="F39" s="108">
         <v>1873.499560122021</v>
       </c>
     </row>
@@ -6495,7 +6551,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="35">
+      <c r="F40" s="38">
         <v>2479.849226425816</v>
       </c>
     </row>
@@ -6515,8 +6571,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="116">
-        <v>141.7841065426883</v>
+      <c r="F41" s="125">
+        <v>112.6021024554471</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6535,8 +6591,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="117">
-        <v>500.6682095047611</v>
+      <c r="F42" s="15">
+        <v>520.6971392210378</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6555,8 +6611,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="118">
-        <v>834.8901557121877</v>
+      <c r="F43" s="126">
+        <v>856.8805061567789</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6575,8 +6631,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="109">
-        <v>32.9243005190282</v>
+      <c r="F44" s="12">
+        <v>46.64822146439845</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6595,8 +6651,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="110">
-        <v>102.5022070381353</v>
+      <c r="F45" s="3">
+        <v>173.6361852044211</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6615,8 +6671,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="20">
-        <v>68.80758320653729</v>
+      <c r="F46" s="110">
+        <v>99.46666229937964</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6635,8 +6691,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="109">
-        <v>36.50989849310458</v>
+      <c r="F47" s="11">
+        <v>36.5098984904831</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6656,7 +6712,7 @@
         <v>14</v>
       </c>
       <c r="F48" s="7">
-        <v>134.2905711595562</v>
+        <v>134.2905708604081</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6675,8 +6731,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="102">
-        <v>82.24745876379453</v>
+      <c r="F49" s="112">
+        <v>82.24745863058621</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6695,7 +6751,7 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="119">
+      <c r="F50" s="127">
         <v>203.3085743149552</v>
       </c>
     </row>
@@ -6715,7 +6771,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="98">
+      <c r="F51" s="128">
         <v>715.5014516919969</v>
       </c>
     </row>
@@ -6735,7 +6791,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="120">
+      <c r="F52" s="129">
         <v>908.2024087334084</v>
       </c>
     </row>
@@ -6755,8 +6811,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="20">
-        <v>77.17497435839286</v>
+      <c r="F53" s="12">
+        <v>41.40679992751784</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6775,8 +6831,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="121">
-        <v>332.7568242642446</v>
+      <c r="F54" s="130">
+        <v>345.00199111353</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6795,8 +6851,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="115">
-        <v>277.3016052957108</v>
+      <c r="F55" s="113">
+        <v>302.5164082971891</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6815,8 +6871,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="11">
-        <v>10.52065291011232</v>
+      <c r="F56" s="18">
+        <v>15.42567752621673</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6835,8 +6891,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="122">
-        <v>66.19990381458774</v>
+      <c r="F57" s="125">
+        <v>109.559330654955</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6855,8 +6911,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="10">
-        <v>41.62982713791985</v>
+      <c r="F58" s="17">
+        <v>56.80852003835454</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6875,8 +6931,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="11">
-        <v>10.74941146605935</v>
+      <c r="F59" s="18">
+        <v>10.74941146343787</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6895,8 +6951,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="102">
-        <v>85.59946363447793</v>
+      <c r="F60" s="112">
+        <v>85.5994633353298</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6915,8 +6971,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="10">
-        <v>46.50818173791374</v>
+      <c r="F61" s="12">
+        <v>46.5081816047054</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6955,7 +7011,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="119">
+      <c r="F63" s="127">
         <v>198.6769964578388</v>
       </c>
     </row>
@@ -6975,7 +7031,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="102">
+      <c r="F64" s="112">
         <v>79.96340726237918</v>
       </c>
     </row>
@@ -6996,7 +7052,7 @@
         <v>11</v>
       </c>
       <c r="F65" s="9">
-        <v>0.1834626616105195</v>
+        <v>0.1820622210973538</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -7015,8 +7071,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="102">
-        <v>81.29373680669678</v>
+      <c r="F66" s="12">
+        <v>46.27138301571736</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -7035,8 +7091,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="11">
-        <v>13.30665948623112</v>
+      <c r="F67" s="9">
+        <v>2.246918086020362</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -7056,7 +7112,7 @@
         <v>11</v>
       </c>
       <c r="F68" s="9">
-        <v>0.1830272760493846</v>
+        <v>0.182552994935995</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -7076,7 +7132,7 @@
         <v>14</v>
       </c>
       <c r="F69" s="9">
-        <v>0.5372370455020633</v>
+        <v>3.172390578078132</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7096,7 +7152,7 @@
         <v>15</v>
       </c>
       <c r="F70" s="9">
-        <v>2.257844340878407</v>
+        <v>2.247809531160659</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -7116,7 +7172,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="9">
-        <v>0.1414736192097876</v>
+        <v>0.1414736227542157</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -7136,7 +7192,7 @@
         <v>14</v>
       </c>
       <c r="F72" s="9">
-        <v>0.4956833886624665</v>
+        <v>0.4956833922068945</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -7156,7 +7212,7 @@
         <v>15</v>
       </c>
       <c r="F73" s="9">
-        <v>1.973204017953146</v>
+        <v>1.973204032884826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed SLB outflows bug
</commit_message>
<xml_diff>
--- a/results/Manuscript/material_use.xlsx
+++ b/results/Manuscript/material_use.xlsx
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="130">
+  <fills count="137">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,25 +120,631 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF4DCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6ADAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EAEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DADA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CFCF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E5E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EFEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E2E2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5CBCB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B9B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EBEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4DBDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E8E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E1E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C8C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B7B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF4E0E0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5C8C8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6B9B9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EEEE"/>
+        <fgColor rgb="FFF4D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E9E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD2F2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE1313"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4040"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD3131"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD2828"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4343"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3D3D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3F3F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4141"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3636"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD1E1E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE0F0F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3434"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD2E2E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3E3E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE1B1B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE0B0B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC3838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4444"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0DEC0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDDCBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1DFC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDDDBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC2DFC2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBEDDBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFDEBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8E2C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAE3CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCDE5CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3E7D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEDDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF3EB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3E0C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF048204"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF058205"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF028102"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF068306"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0C860C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF108810"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF158A15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF188C18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF289328"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3D9E3D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF038103"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF128912"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E0C5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD5AD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4D0A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5F0E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFEDDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAF2EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6F1E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9CCD9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF73B873"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF45A245"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD6AF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4F0E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EEE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EEDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCDCBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF83C083"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4E8D4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EC58E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF51A851"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EEE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1E6D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81BF81"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3EFE3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F1E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D6D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79797"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97373"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,25 +756,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4DBDB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EAEA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EDED"/>
+        <fgColor rgb="FFF5BCBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C4C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C6C6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D4D4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C7C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97C7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB4646"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79D9D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF88181"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C9C9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D8D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4D7D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79696"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97575"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3E3E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79F9F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5CACA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,577 +864,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4E1E1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5CBCB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5BEBE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DCDC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EBEB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EFEF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5CCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6AAAA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF89090"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C4C4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E8E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E9E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA6060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4848"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC3939"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97070"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA6868"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97171"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF96F6F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97272"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4A4A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC3B3B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA5E5E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4C4C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFD2121"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF96D6D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8FC68F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8CC58C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8BC48B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8DC58D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90C790"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BCC9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA2CFA2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA6D2A6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF91C791"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95C995"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8DAB8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1E6D1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF3EB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99CB99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA1CFA1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBCDCBC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94C994"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ACB9A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF98CA98"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF97CA97"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF038103"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF058205"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF028102"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF068306"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF138913"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1D8E1D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF289328"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF128912"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2E972E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF56AA56"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CBD7C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF098509"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF178B17"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF339933"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0A850A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF088408"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF078407"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC2DFC2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA3D0A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92C892"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6F1E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFE2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD4E8D4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9F2E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7F1E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2E8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ECE9E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF69B369"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF349A34"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDCECDC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC8E2C8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5F0E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAEBDA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8EAD8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDECDD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDFEDDF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6DB66D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1EEE1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBDCBB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEAF2EA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4AA44A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE4F0E4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7E1C7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0EEE0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE3EFE3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7A3A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC3A3A"/>
+        <fgColor rgb="FFF4D2D2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,127 +882,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3E7E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D7D7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E8E8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DEDE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D5D5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79B9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF97777"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6B8B7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DFDF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E5E5"/>
+        <fgColor rgb="FFF4DDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF88585"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA5959"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B3B3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7A4A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79898"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5C5C5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5BFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DADA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3E6E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79D9D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4DDDD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6ABAB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79898"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CFCF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -914,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -942,10 +984,10 @@
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -957,16 +999,16 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -978,9 +1020,9 @@
     <xf numFmtId="0" fontId="2" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -989,13 +1031,13 @@
     <xf numFmtId="0" fontId="3" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="75" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="78" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="79" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="80" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1004,10 +1046,10 @@
     <xf numFmtId="0" fontId="2" fillId="83" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="84" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="85" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="90" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="91" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="92" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1019,35 +1061,42 @@
     <xf numFmtId="0" fontId="2" fillId="98" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="99" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="100" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="102" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="103" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="104" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="105" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="106" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="106" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="109" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="110" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="111" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="112" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="113" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="114" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="113" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="114" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="115" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="116" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="117" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="118" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="119" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="120" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="121" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="121" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="122" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="123" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="124" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="125" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="126" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="127" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="128" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="128" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="129" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="130" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="131" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="132" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="133" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="134" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="135" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="136" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,7 +1431,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="3">
-        <v>38042.81187722955</v>
+        <v>31308.50288468429</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1402,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="4">
-        <v>38997.70339404551</v>
+        <v>32116.77185932662</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1422,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="5">
-        <v>39590.61940778202</v>
+        <v>32652.77289356306</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1442,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="6">
-        <v>37498.43080197114</v>
+        <v>30913.20617542131</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1462,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="7">
-        <v>37902.63267189218</v>
+        <v>31386.85172422463</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1482,7 +1531,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="8">
-        <v>38231.43766327716</v>
+        <v>31692.99736956487</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1502,7 +1551,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="9">
-        <v>37410.71985159518</v>
+        <v>30806.71551505055</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1522,7 +1571,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="10">
-        <v>37621.04873812848</v>
+        <v>31092.20905234555</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1542,7 +1591,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="11">
-        <v>37537.15574481436</v>
+        <v>31045.04873313245</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1561,8 +1610,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="9">
-        <v>37395.5408395745</v>
+      <c r="F11" s="12">
+        <v>30789.84472166983</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1581,8 +1630,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="12">
-        <v>37559.45118173854</v>
+      <c r="F12" s="13">
+        <v>31019.23683556635</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1602,7 +1651,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="6">
-        <v>37472.21420624205</v>
+        <v>30922.13638687821</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1621,8 +1670,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="13">
-        <v>38027.6536108783</v>
+      <c r="F14" s="14">
+        <v>31146.64635002538</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1641,8 +1690,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="14">
-        <v>38862.37038121407</v>
+      <c r="F15" s="15">
+        <v>31815.96380544874</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1661,8 +1710,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="15">
-        <v>39409.03516301885</v>
+      <c r="F16" s="16">
+        <v>32316.02656635926</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1681,8 +1730,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="6">
-        <v>37489.88472757782</v>
+      <c r="F17" s="17">
+        <v>30884.54208234422</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1701,8 +1750,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="7">
-        <v>37887.37253452981</v>
+      <c r="F18" s="18">
+        <v>31336.20746375139</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1721,8 +1770,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="16">
-        <v>38200.3933659232</v>
+      <c r="F19" s="19">
+        <v>31585.36554283437</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1741,8 +1790,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="9">
-        <v>37402.82638715756</v>
+      <c r="F20" s="12">
+        <v>30790.92900117916</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1761,8 +1810,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="17">
-        <v>37610.51451471172</v>
+      <c r="F21" s="11">
+        <v>31063.53761786732</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1781,8 +1830,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="11">
-        <v>37527.02778757971</v>
+      <c r="F22" s="20">
+        <v>31003.25397522288</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1801,8 +1850,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="9">
-        <v>37389.50869061065</v>
+      <c r="F23" s="12">
+        <v>30776.37656152951</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1821,8 +1870,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="12">
-        <v>37552.30761752666</v>
+      <c r="F24" s="20">
+        <v>30996.60895870821</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1841,8 +1890,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="18">
-        <v>37463.17788638971</v>
+      <c r="F25" s="17">
+        <v>30893.46495239998</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1861,8 +1910,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="19">
-        <v>38820.09493073855</v>
+      <c r="F26" s="21">
+        <v>31180.57531405703</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1881,8 +1930,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="20">
-        <v>40176.08684177568</v>
+      <c r="F27" s="22">
+        <v>31911.46094542385</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1901,8 +1950,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="21">
-        <v>41241.89777610592</v>
+      <c r="F28" s="23">
+        <v>32392.8249820646</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1921,8 +1970,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="17">
-        <v>37612.86830548158</v>
+      <c r="F29" s="9">
+        <v>30816.77261055443</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1941,8 +1990,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="16">
-        <v>38209.37177112736</v>
+      <c r="F30" s="24">
+        <v>31212.17635286283</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1961,8 +2010,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="22">
-        <v>39179.1577698071</v>
+      <c r="F31" s="25">
+        <v>31401.05439593284</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1981,8 +2030,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="18">
-        <v>37448.38755813866</v>
+      <c r="F32" s="26">
+        <v>30756.35708700759</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2001,8 +2050,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="23">
-        <v>37740.03366767087</v>
+      <c r="F33" s="20">
+        <v>30992.39626055396</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2021,8 +2070,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="24">
-        <v>37686.53228787622</v>
+      <c r="F34" s="6">
+        <v>30905.80716637464</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2041,8 +2090,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="18">
-        <v>37427.7530300599</v>
+      <c r="F35" s="26">
+        <v>30744.80091826475</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2061,8 +2110,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="24">
-        <v>37658.53375119837</v>
+      <c r="F36" s="27">
+        <v>30937.16462655976</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2081,8 +2130,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="12">
-        <v>37561.84975889421</v>
+      <c r="F37" s="28">
+        <v>30833.47822897095</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2101,8 +2150,8 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="25">
-        <v>43146.87751981514</v>
+      <c r="F38" s="29">
+        <v>36256.53938489911</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2121,8 +2170,8 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="26">
-        <v>44101.76903663111</v>
+      <c r="F39" s="30">
+        <v>37064.80835954143</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2141,8 +2190,8 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="27">
-        <v>44694.68505036762</v>
+      <c r="F40" s="31">
+        <v>37600.80939377788</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2161,8 +2210,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="28">
-        <v>42520.59871654321</v>
+      <c r="F41" s="32">
+        <v>35774.42325736617</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2181,8 +2230,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="29">
-        <v>42840.58392931787</v>
+      <c r="F42" s="33">
+        <v>36195.04654896527</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2201,8 +2250,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="25">
-        <v>43175.26330096238</v>
+      <c r="F43" s="34">
+        <v>36465.35890463279</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2221,8 +2270,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="30">
-        <v>42470.88661173557</v>
+      <c r="F44" s="35">
+        <v>35698.26219215386</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2241,8 +2290,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="31">
-        <v>42565.16501139421</v>
+      <c r="F45" s="36">
+        <v>35842.4653293194</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2261,8 +2310,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="28">
-        <v>42509.63678944725</v>
+      <c r="F46" s="32">
+        <v>35754.67382064828</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2281,8 +2330,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="32">
-        <v>42463.42532364507</v>
+      <c r="F47" s="35">
+        <v>35690.26741098692</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2301,8 +2350,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="28">
-        <v>42535.51332053153</v>
+      <c r="F48" s="37">
+        <v>35795.29729106486</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2321,8 +2370,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="30">
-        <v>42496.8518928113</v>
+      <c r="F49" s="38">
+        <v>35732.95856953711</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2341,8 +2390,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="25">
-        <v>43174.29827220868</v>
+      <c r="F50" s="39">
+        <v>36073.00908997656</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2361,8 +2410,8 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="33">
-        <v>44042.88994517744</v>
+      <c r="F51" s="40">
+        <v>36723.10399304463</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2381,8 +2430,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="34">
-        <v>44632.76660394678</v>
+      <c r="F52" s="41">
+        <v>37167.17222309698</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2401,8 +2450,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="28">
-        <v>42508.61373339163</v>
+      <c r="F53" s="38">
+        <v>35748.64622170095</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2421,8 +2470,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="29">
-        <v>42810.90772176443</v>
+      <c r="F54" s="42">
+        <v>36121.54746040817</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2441,8 +2490,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="35">
-        <v>43223.79136664226</v>
+      <c r="F55" s="43">
+        <v>36273.04811355958</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2461,8 +2510,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="30">
-        <v>42464.8913964779</v>
+      <c r="F56" s="35">
+        <v>35689.30527738567</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2481,8 +2530,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="31">
-        <v>42552.94645746489</v>
+      <c r="F57" s="44">
+        <v>35821.50441018996</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2501,8 +2550,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="28">
-        <v>42501.77369760885</v>
+      <c r="F58" s="38">
+        <v>35739.77251162053</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2521,8 +2570,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="32">
-        <v>42458.78580141172</v>
+      <c r="F59" s="35">
+        <v>35683.08917375551</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2541,8 +2590,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="28">
-        <v>42525.5570404518</v>
+      <c r="F60" s="37">
+        <v>35780.39598203712</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2561,8 +2610,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="30">
-        <v>42489.33497618809</v>
+      <c r="F61" s="45">
+        <v>35722.52643684297</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2581,8 +2630,8 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="36">
-        <v>43964.38010005821</v>
+      <c r="F62" s="42">
+        <v>36109.24617364286</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2601,8 +2650,8 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="37">
-        <v>45673.59602566905</v>
+      <c r="F63" s="46">
+        <v>36820.49428274581</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2621,8 +2670,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="38">
-        <v>47012.52701914091</v>
+      <c r="F64" s="47">
+        <v>37264.94123621205</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2641,8 +2690,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="31">
-        <v>42566.92361934109</v>
+      <c r="F65" s="45">
+        <v>35699.56192846098</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2661,8 +2710,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="25">
-        <v>43145.31036802677</v>
+      <c r="F66" s="48">
+        <v>35982.27288317835</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2681,8 +2730,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="26">
-        <v>44138.37101440705</v>
+      <c r="F67" s="33">
+        <v>36184.5958639324</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2701,8 +2750,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="30">
-        <v>42485.48141090687</v>
+      <c r="F68" s="49">
+        <v>35670.85707168161</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2721,8 +2770,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="39">
-        <v>42621.29943980042</v>
+      <c r="F69" s="32">
+        <v>35774.94540698842</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2741,8 +2790,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="31">
-        <v>42545.97011032965</v>
+      <c r="F70" s="45">
+        <v>35710.42293570488</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2761,8 +2810,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="30">
-        <v>42476.0153870825</v>
+      <c r="F71" s="49">
+        <v>35666.91057440764</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2781,8 +2830,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="31">
-        <v>42576.14125754007</v>
+      <c r="F72" s="38">
+        <v>35743.6253293506</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2801,8 +2850,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="28">
-        <v>42524.91536559458</v>
+      <c r="F73" s="45">
+        <v>35699.69372485037</v>
       </c>
     </row>
   </sheetData>
@@ -2851,8 +2900,8 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="40">
-        <v>7526.317007325268</v>
+      <c r="F2" s="50">
+        <v>3484.710325762061</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2871,8 +2920,8 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="41">
-        <v>7641.74377550096</v>
+      <c r="F3" s="51">
+        <v>3543.90197031129</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2891,8 +2940,8 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="42">
-        <v>7655.177428068251</v>
+      <c r="F4" s="51">
+        <v>3535.506478756357</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2911,8 +2960,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="40">
-        <v>7485.283081260031</v>
+      <c r="F5" s="52">
+        <v>3470.743020189666</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2931,8 +2980,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="43">
-        <v>7587.658791039436</v>
+      <c r="F6" s="53">
+        <v>3528.214422379022</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2951,8 +3000,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="43">
-        <v>7594.339770659917</v>
+      <c r="F7" s="53">
+        <v>3519.123734929587</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2971,8 +3020,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="44">
-        <v>7460.618440913315</v>
+      <c r="F8" s="54">
+        <v>3457.144395896106</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2991,8 +3040,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="40">
-        <v>7525.584462536903</v>
+      <c r="F9" s="55">
+        <v>3504.303417556111</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3011,8 +3060,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40">
-        <v>7498.378400995356</v>
+      <c r="F10" s="56">
+        <v>3488.598575254351</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3031,8 +3080,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="44">
-        <v>7455.714864042428</v>
+      <c r="F11" s="54">
+        <v>3454.085857509751</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3051,8 +3100,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="40">
-        <v>7508.886192658765</v>
+      <c r="F12" s="56">
+        <v>3496.048014208128</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3071,8 +3120,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="40">
-        <v>7481.233153735411</v>
+      <c r="F13" s="50">
+        <v>3477.805261532034</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3091,8 +3140,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="45">
-        <v>7024.441944697281</v>
+      <c r="F14" s="57">
+        <v>3365.525376545845</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3111,8 +3160,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="46">
-        <v>6783.149043639318</v>
+      <c r="F15" s="58">
+        <v>3319.822853242871</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3131,8 +3180,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="47">
-        <v>6608.194684521932</v>
+      <c r="F16" s="59">
+        <v>3283.023171932641</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3151,8 +3200,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48">
-        <v>7410.456130585966</v>
+      <c r="F17" s="52">
+        <v>3465.95139037666</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3171,8 +3220,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="44">
-        <v>7465.797623001579</v>
+      <c r="F18" s="53">
+        <v>3522.615692441332</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3191,8 +3240,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="49">
-        <v>7291.101151940789</v>
+      <c r="F19" s="55">
+        <v>3509.680023834399</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3211,8 +3260,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="48">
-        <v>7416.477715263414</v>
+      <c r="F20" s="54">
+        <v>3453.5168879982</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3231,8 +3280,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="44">
-        <v>7459.067986028058</v>
+      <c r="F21" s="56">
+        <v>3499.519129144252</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3251,8 +3300,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="48">
-        <v>7420.578682158948</v>
+      <c r="F22" s="50">
+        <v>3483.239929932843</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3271,8 +3320,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="48">
-        <v>7419.599452738314</v>
+      <c r="F23" s="54">
+        <v>3450.762577828581</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3291,8 +3340,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="44">
-        <v>7452.515101727635</v>
+      <c r="F24" s="56">
+        <v>3491.695574065511</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3311,8 +3360,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="48">
-        <v>7426.754818444741</v>
+      <c r="F25" s="52">
+        <v>3473.020973120175</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3331,8 +3380,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="50">
-        <v>5972.38224728867</v>
+      <c r="F26" s="60">
+        <v>3192.24895844635</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3351,8 +3400,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="51">
-        <v>5037.127154289265</v>
+      <c r="F27" s="61">
+        <v>3010.769844526417</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3371,8 +3420,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="52">
-        <v>4035.335950068962</v>
+      <c r="F28" s="62">
+        <v>2804.962583936494</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3391,8 +3440,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="53">
-        <v>7153.079303942879</v>
+      <c r="F29" s="54">
+        <v>3453.450055161019</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3411,8 +3460,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="54">
-        <v>6839.923419658385</v>
+      <c r="F30" s="55">
+        <v>3507.149292616679</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3431,8 +3480,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="55">
-        <v>5813.728243882939</v>
+      <c r="F31" s="63">
+        <v>3444.107039405113</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3451,8 +3500,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="56">
-        <v>7317.560051285805</v>
+      <c r="F32" s="63">
+        <v>3444.638195980279</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3471,8 +3520,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="53">
-        <v>7142.294514734924</v>
+      <c r="F33" s="50">
+        <v>3486.846415053501</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3491,8 +3540,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="57">
-        <v>7093.57160599095</v>
+      <c r="F34" s="52">
+        <v>3468.919505351642</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3511,8 +3560,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="58">
-        <v>7338.19457936457</v>
+      <c r="F35" s="63">
+        <v>3442.428006329992</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3531,8 +3580,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="59">
-        <v>7187.485295435928</v>
+      <c r="F36" s="50">
+        <v>3479.940186402973</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3551,8 +3600,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="60">
-        <v>7209.490293347926</v>
+      <c r="F37" s="52">
+        <v>3461.139993137626</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3571,8 +3620,8 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="61">
-        <v>12788.24710269182</v>
+      <c r="F38" s="64">
+        <v>6468.944523086681</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3591,8 +3640,8 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="62">
-        <v>12903.67387086751</v>
+      <c r="F39" s="65">
+        <v>6528.136167635911</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3611,8 +3660,8 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="62">
-        <v>12917.1075234348</v>
+      <c r="F40" s="65">
+        <v>6519.740676080978</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3631,8 +3680,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="63">
-        <v>12723.94673328884</v>
+      <c r="F41" s="66">
+        <v>6443.368727644604</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3651,8 +3700,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="61">
-        <v>12812.05655727977</v>
+      <c r="F42" s="67">
+        <v>6498.121172315093</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3671,8 +3720,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="64">
-        <v>12813.56055257101</v>
+      <c r="F43" s="67">
+        <v>6488.452412941041</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3691,8 +3740,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="65">
-        <v>12707.70495710543</v>
+      <c r="F44" s="68">
+        <v>6429.926877809849</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3711,8 +3760,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="63">
-        <v>12740.41452118682</v>
+      <c r="F45" s="64">
+        <v>6461.432730005864</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3731,8 +3780,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="63">
-        <v>12721.77322022874</v>
+      <c r="F46" s="66">
+        <v>6444.537014765306</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3751,8 +3800,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="65">
-        <v>12705.02792222202</v>
+      <c r="F47" s="68">
+        <v>6427.909163473668</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3771,8 +3820,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="63">
-        <v>12730.72059770548</v>
+      <c r="F48" s="66">
+        <v>6453.33368453079</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3791,8 +3840,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="63">
-        <v>12717.33891319589</v>
+      <c r="F49" s="68">
+        <v>6440.049589534577</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3811,8 +3860,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="66">
-        <v>12160.95364948288</v>
+      <c r="F50" s="69">
+        <v>6333.98025305154</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3831,8 +3880,8 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="67">
-        <v>11804.55485389116</v>
+      <c r="F51" s="70">
+        <v>6273.178672176423</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3851,8 +3900,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="68">
-        <v>11407.37915216324</v>
+      <c r="F52" s="71">
+        <v>6192.049555804933</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3871,8 +3920,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="65">
-        <v>12664.7364139125</v>
+      <c r="F53" s="68">
+        <v>6438.605884320655</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3891,8 +3940,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="65">
-        <v>12666.03761672571</v>
+      <c r="F54" s="67">
+        <v>6486.997967098915</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3911,8 +3960,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="69">
-        <v>12210.66838903153</v>
+      <c r="F55" s="64">
+        <v>6460.933937693825</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3931,8 +3980,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="65">
-        <v>12682.47762842492</v>
+      <c r="F56" s="68">
+        <v>6427.458397286663</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3951,8 +4000,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="65">
-        <v>12688.55622056666</v>
+      <c r="F57" s="64">
+        <v>6457.144149006678</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3971,8 +4020,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="65">
-        <v>12686.97816980611</v>
+      <c r="F58" s="66">
+        <v>6441.031911473267</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3991,8 +4040,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="65">
-        <v>12683.90695742833</v>
+      <c r="F59" s="68">
+        <v>6425.804576072384</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4011,8 +4060,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="65">
-        <v>12691.98577026014</v>
+      <c r="F60" s="66">
+        <v>6449.828581238752</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -4031,8 +4080,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="65">
-        <v>12689.11655279322</v>
+      <c r="F61" s="68">
+        <v>6437.282860121452</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4051,8 +4100,8 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="70">
-        <v>11167.74671002897</v>
+      <c r="F62" s="72">
+        <v>6137.77604724048</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -4071,8 +4120,8 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="71">
-        <v>9657.024318165388</v>
+      <c r="F63" s="73">
+        <v>5899.647333218948</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -4091,8 +4140,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="72">
-        <v>8199.379735498071</v>
+      <c r="F64" s="74">
+        <v>5567.108640947386</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -4111,8 +4160,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="73">
-        <v>12565.20179025661</v>
+      <c r="F65" s="68">
+        <v>6427.776289282663</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4131,8 +4180,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="74">
-        <v>12032.90436236553</v>
+      <c r="F66" s="75">
+        <v>6471.164703497296</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4151,8 +4200,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="75">
-        <v>10995.81925105556</v>
+      <c r="F67" s="76">
+        <v>6229.161799775409</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4171,8 +4220,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="65">
-        <v>12646.64448946467</v>
+      <c r="F68" s="68">
+        <v>6421.891384087424</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4191,8 +4240,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="76">
-        <v>12513.81629815426</v>
+      <c r="F69" s="66">
+        <v>6446.719761147539</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4211,8 +4260,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="77">
-        <v>12588.2210465781</v>
+      <c r="F70" s="68">
+        <v>6433.268314398474</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4231,8 +4280,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="65">
-        <v>12656.06943391686</v>
+      <c r="F71" s="68">
+        <v>6420.816498931807</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4251,8 +4300,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="73">
-        <v>12556.29777322873</v>
+      <c r="F72" s="68">
+        <v>6440.825226581551</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4271,8 +4320,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="78">
-        <v>12609.0011858149</v>
+      <c r="F73" s="68">
+        <v>6430.809294465103</v>
       </c>
     </row>
   </sheetData>
@@ -4321,7 +4370,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4341,7 +4390,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4361,7 +4410,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4381,7 +4430,7 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4401,7 +4450,7 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4421,7 +4470,7 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4441,7 +4490,7 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4461,7 +4510,7 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4481,7 +4530,7 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4501,7 +4550,7 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4521,7 +4570,7 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4541,7 +4590,7 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4561,8 +4610,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="79">
-        <v>1650.829858861342</v>
+      <c r="F14" s="77">
+        <v>776.947283782711</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4581,8 +4630,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="80">
-        <v>2881.854852240659</v>
+      <c r="F15" s="78">
+        <v>1269.268698901808</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4601,8 +4650,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="81">
-        <v>3533.499652148049</v>
+      <c r="F16" s="79">
+        <v>1453.322957496987</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -4621,8 +4670,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="82">
-        <v>195.6104432047388</v>
+      <c r="F17" s="80">
+        <v>65.64504150066757</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4641,8 +4690,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="83">
-        <v>336.9535906915762</v>
+      <c r="F18" s="81">
+        <v>115.7436736172667</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4661,8 +4710,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="84">
-        <v>949.6895523472003</v>
+      <c r="F19" s="82">
+        <v>252.5413318475803</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4681,8 +4730,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="85">
-        <v>108.8522090549048</v>
+      <c r="F20" s="83">
+        <v>35.14205846374063</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4701,8 +4750,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="86">
-        <v>169.9460619159358</v>
+      <c r="F21" s="80">
+        <v>61.74191367827886</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4721,8 +4770,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="82">
-        <v>203.4457937514989</v>
+      <c r="F22" s="84">
+        <v>94.32298192994938</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4741,8 +4790,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="85">
-        <v>88.73523084425588</v>
+      <c r="F23" s="83">
+        <v>28.50547413855713</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4761,8 +4810,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="87">
-        <v>143.290171861868</v>
+      <c r="F24" s="85">
+        <v>48.43026831801955</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4781,8 +4830,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="87">
-        <v>136.6083246091488</v>
+      <c r="F25" s="80">
+        <v>61.74191367827886</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4801,8 +4850,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="88">
-        <v>3084.46527939775</v>
+      <c r="F26" s="86">
+        <v>1592.826201500888</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -4821,8 +4870,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="89">
-        <v>5218.548969676591</v>
+      <c r="F27" s="87">
+        <v>2447.834162260545</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4841,8 +4890,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="90">
-        <v>7290.550607051456</v>
+      <c r="F28" s="88">
+        <v>3373.704118274395</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4861,8 +4910,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="91">
-        <v>606.084637217702</v>
+      <c r="F29" s="61">
+        <v>274.6957403372998</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4881,8 +4930,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="92">
-        <v>1405.663904701903</v>
+      <c r="F30" s="60">
+        <v>487.4769334659765</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4901,8 +4950,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="58">
-        <v>3506.802908930157</v>
+      <c r="F31" s="89">
+        <v>1222.353167712925</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4921,8 +4970,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="93">
-        <v>254.0593554738107</v>
+      <c r="F32" s="90">
+        <v>139.6147085749215</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4941,8 +4990,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="94">
-        <v>693.7358982401573</v>
+      <c r="F33" s="82">
+        <v>255.8723450537753</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4961,8 +5010,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="95">
-        <v>744.1541077626994</v>
+      <c r="F34" s="91">
+        <v>373.0471275236956</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4981,8 +5030,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="82">
-        <v>209.2314851255441</v>
+      <c r="F35" s="81">
+        <v>118.0672363215096</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -5001,8 +5050,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="96">
-        <v>579.5182345907845</v>
+      <c r="F36" s="92">
+        <v>207.3667693909634</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -5021,8 +5070,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="97">
-        <v>492.5213881821418</v>
+      <c r="F37" s="93">
+        <v>242.5134724461028</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -5041,7 +5090,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="52">
+      <c r="F38" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5061,7 +5110,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="52">
+      <c r="F39" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5081,7 +5130,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5101,7 +5150,7 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="52">
+      <c r="F41" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5121,7 +5170,7 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="52">
+      <c r="F42" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5141,7 +5190,7 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="52">
+      <c r="F43" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5161,7 +5210,7 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="52">
+      <c r="F44" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5181,7 +5230,7 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="52">
+      <c r="F45" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5201,7 +5250,7 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="52">
+      <c r="F46" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5221,7 +5270,7 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5241,7 +5290,7 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="52">
+      <c r="F48" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5261,7 +5310,7 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="52">
+      <c r="F49" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5281,8 +5330,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="50">
-        <v>2033.809028558813</v>
+      <c r="F50" s="94">
+        <v>957.4485125771901</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5301,8 +5350,8 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="44">
-        <v>3628.26835827906</v>
+      <c r="F51" s="86">
+        <v>1593.743821344552</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -5321,8 +5370,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="98">
-        <v>5019.446721344348</v>
+      <c r="F52" s="95">
+        <v>2130.826243049877</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5341,8 +5390,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="86">
-        <v>149.1270711280139</v>
+      <c r="F53" s="85">
+        <v>53.19532017783293</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -5361,8 +5410,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="99">
-        <v>395.269390458085</v>
+      <c r="F54" s="90">
+        <v>144.9819274179409</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5381,8 +5430,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="100">
-        <v>1922.706280258855</v>
+      <c r="F55" s="96">
+        <v>475.2447748072078</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5401,8 +5450,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="101">
-        <v>61.19266001313503</v>
+      <c r="F56" s="83">
+        <v>18.91098768620373</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5421,8 +5470,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="87">
-        <v>128.2441842873131</v>
+      <c r="F57" s="85">
+        <v>41.61902234569372</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5441,8 +5490,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="85">
-        <v>85.19809325586476</v>
+      <c r="F58" s="83">
+        <v>29.80130598904827</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5461,8 +5510,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="101">
-        <v>51.51758754533567</v>
+      <c r="F59" s="62">
+        <v>14.50186217095843</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5481,8 +5530,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="85">
-        <v>93.97536146749252</v>
+      <c r="F60" s="83">
+        <v>29.80130598904827</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -5501,8 +5550,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="101">
-        <v>67.75408785841486</v>
+      <c r="F61" s="83">
+        <v>20.98905050705926</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -5521,8 +5570,8 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="45">
-        <v>3209.189600955568</v>
+      <c r="F62" s="97">
+        <v>1902.008445514517</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -5541,8 +5590,8 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="102">
-        <v>6452.649325876972</v>
+      <c r="F63" s="98">
+        <v>3137.568933481597</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -5561,8 +5610,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="62">
-        <v>9411.587846975366</v>
+      <c r="F64" s="65">
+        <v>4794.007511144423</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5581,8 +5630,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="103">
-        <v>289.4256474956678</v>
+      <c r="F65" s="99">
+        <v>194.037687052477</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5601,8 +5650,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="104">
-        <v>1464.817806165867</v>
+      <c r="F66" s="100">
+        <v>526.34686842519</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5621,8 +5670,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="48">
-        <v>3583.372124797327</v>
+      <c r="F67" s="101">
+        <v>2172.225846674564</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5641,8 +5690,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="85">
-        <v>110.0044816763576</v>
+      <c r="F68" s="80">
+        <v>71.38856286543295</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -5661,8 +5710,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="105">
-        <v>407.8904046906079</v>
+      <c r="F69" s="102">
+        <v>161.4407194325501</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5681,8 +5730,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="93">
-        <v>242.8329589295964</v>
+      <c r="F70" s="84">
+        <v>109.9446947539117</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -5701,8 +5750,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="85">
-        <v>88.79171035304222</v>
+      <c r="F71" s="80">
+        <v>57.88515169447861</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -5721,8 +5770,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="106">
-        <v>312.6598809927535</v>
+      <c r="F72" s="81">
+        <v>122.7558413406463</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -5741,8 +5790,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="82">
-        <v>196.4518343454459</v>
+      <c r="F73" s="103">
+        <v>81.9630919655703</v>
       </c>
     </row>
   </sheetData>
@@ -5791,8 +5840,8 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="107">
-        <v>803.1812751303619</v>
+      <c r="F2" s="104">
+        <v>657.338309439164</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5811,8 +5860,8 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="108">
-        <v>1873.499560122021</v>
+      <c r="F3" s="44">
+        <v>1524.798928630718</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5831,8 +5880,8 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="38">
-        <v>2479.849226425816</v>
+      <c r="F4" s="31">
+        <v>2052.404471312229</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5851,8 +5900,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8">
-        <v>217.7662738067129</v>
+      <c r="F5" s="105">
+        <v>248.0742946037855</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5871,8 +5920,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="20">
-        <v>724.343853507159</v>
+      <c r="F6" s="106">
+        <v>779.1912455964575</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5891,8 +5940,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="109">
-        <v>1059.829824512622</v>
+      <c r="F7" s="107">
+        <v>1076.246203487269</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5911,8 +5960,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="110">
-        <v>105.3906830840426</v>
+      <c r="F8" s="108">
+        <v>127.9850099394693</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5931,8 +5980,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="14">
-        <v>380.6855912409278</v>
+      <c r="F9" s="109">
+        <v>460.6375688944728</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5951,8 +6000,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="111">
-        <v>269.5865363852637</v>
+      <c r="F10" s="110">
+        <v>397.7724073796143</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5971,8 +6020,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="112">
-        <v>85.30809419247382</v>
+      <c r="F11" s="11">
+        <v>108.0556781723916</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5991,8 +6040,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="113">
-        <v>302.3897649728449</v>
+      <c r="F12" s="111">
+        <v>379.4099487672818</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6011,8 +6060,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="114">
-        <v>187.4997505530028</v>
+      <c r="F13" s="112">
+        <v>264.0667474030532</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6031,8 +6080,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="115">
-        <v>286.1479461511316</v>
+      <c r="F14" s="113">
+        <v>376.2968255640352</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6051,8 +6100,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="116">
-        <v>879.5718154289259</v>
+      <c r="F15" s="114">
+        <v>999.9117576844228</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6071,8 +6120,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="117">
-        <v>1251.282238116325</v>
+      <c r="F16" s="115">
+        <v>1463.174837284711</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -6091,8 +6140,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="7">
-        <v>134.3932487393278</v>
+      <c r="F17" s="25">
+        <v>214.6185717136902</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6111,8 +6160,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="118">
-        <v>587.222548106937</v>
+      <c r="F18" s="116">
+        <v>722.9482551855326</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6131,8 +6180,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="20">
-        <v>725.5469084395307</v>
+      <c r="F19" s="117">
+        <v>959.1706656615809</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6151,8 +6200,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="17">
-        <v>53.3564929965241</v>
+      <c r="F20" s="11">
+        <v>108.5709881701646</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6171,8 +6220,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="113">
-        <v>303.6348913153278</v>
+      <c r="F21" s="4">
+        <v>427.1818460043776</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -6191,8 +6240,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="119">
-        <v>181.6588603142008</v>
+      <c r="F22" s="118">
+        <v>350.6190041485276</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6211,8 +6260,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="12">
-        <v>43.16053392450752</v>
+      <c r="F23" s="20">
+        <v>91.26423835089506</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6231,8 +6280,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="120">
-        <v>238.8751098298445</v>
+      <c r="F24" s="118">
+        <v>352.4296317665307</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6251,8 +6300,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="121">
-        <v>123.9850954100024</v>
+      <c r="F25" s="119">
+        <v>230.6110245129578</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6271,8 +6320,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="6">
-        <v>26.52956860275165</v>
+      <c r="F26" s="120">
+        <v>236.9493714961847</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6291,8 +6340,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="122">
-        <v>447.2663866404827</v>
+      <c r="F27" s="121">
+        <v>786.3558889430577</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6311,8 +6360,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="123">
-        <v>511.2861167504222</v>
+      <c r="F28" s="122">
+        <v>1061.912664993885</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6331,8 +6380,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="9">
-        <v>0</v>
+      <c r="F29" s="123">
+        <v>134.3477647082477</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6351,8 +6400,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="115">
-        <v>283.3475813612906</v>
+      <c r="F30" s="5">
+        <v>583.4507444723068</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6372,7 +6421,7 @@
         <v>15</v>
       </c>
       <c r="F31" s="124">
-        <v>226.9384042655693</v>
+        <v>709.2865343307651</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6391,8 +6440,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="9">
-        <v>0</v>
+      <c r="F32" s="17">
+        <v>65.12038198066942</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -6411,8 +6460,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="121">
-        <v>116.3805729813275</v>
+      <c r="F33" s="125">
+        <v>343.3677746002728</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6431,8 +6480,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="18">
-        <v>14.15628444271354</v>
+      <c r="F34" s="120">
+        <v>238.8517707190812</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6451,8 +6500,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="9">
-        <v>0</v>
+      <c r="F35" s="126">
+        <v>51.3540235875361</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6471,8 +6520,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="112">
-        <v>80.07143720982413</v>
+      <c r="F36" s="127">
+        <v>281.2299119555381</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6491,8 +6540,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="9">
-        <v>5.392442817685369</v>
+      <c r="F37" s="24">
+        <v>158.7433211013739</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6511,8 +6560,8 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="107">
-        <v>803.1812751303619</v>
+      <c r="F38" s="104">
+        <v>657.338309439164</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -6531,8 +6580,8 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="108">
-        <v>1873.499560122021</v>
+      <c r="F39" s="44">
+        <v>1524.798928630718</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -6551,8 +6600,8 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="38">
-        <v>2479.849226425816</v>
+      <c r="F40" s="31">
+        <v>2052.404471312229</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -6571,8 +6620,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="125">
-        <v>112.6021024554471</v>
+      <c r="F41" s="21">
+        <v>149.6463864641597</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6591,8 +6640,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="15">
-        <v>520.6971392210378</v>
+      <c r="F42" s="128">
+        <v>625.0221227337416</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6611,8 +6660,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="126">
-        <v>856.8805061567789</v>
+      <c r="F43" s="129">
+        <v>885.6657190272073</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6631,8 +6680,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="12">
-        <v>46.64822146439845</v>
+      <c r="F44" s="17">
+        <v>60.04347141709579</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6651,8 +6700,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="3">
-        <v>173.6361852044211</v>
+      <c r="F45" s="120">
+        <v>235.7524607786467</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6671,8 +6720,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="110">
-        <v>99.46666229937964</v>
+      <c r="F46" s="123">
+        <v>131.0652368669674</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6691,8 +6740,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="11">
-        <v>36.5098984904831</v>
+      <c r="F47" s="28">
+        <v>50.03097591396831</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6711,8 +6760,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="7">
-        <v>134.2905708604081</v>
+      <c r="F48" s="130">
+        <v>180.4853770490379</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6731,8 +6780,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="112">
-        <v>82.24745863058621</v>
+      <c r="F49" s="13">
+        <v>104.8625605250693</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6751,8 +6800,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="127">
-        <v>203.3085743149552</v>
+      <c r="F50" s="125">
+        <v>338.8437444814808</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -6771,8 +6820,8 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="128">
-        <v>715.5014516919969</v>
+      <c r="F51" s="131">
+        <v>928.1370666744319</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6791,8 +6840,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="129">
-        <v>908.2024087334084</v>
+      <c r="F52" s="132">
+        <v>1291.076180355287</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -6811,8 +6860,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="12">
-        <v>41.40679992751784</v>
+      <c r="F53" s="10">
+        <v>119.1065074749921</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6831,8 +6880,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="130">
-        <v>345.00199111353</v>
+      <c r="F54" s="133">
+        <v>540.3998289604566</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6851,8 +6900,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="113">
-        <v>302.5164082971891</v>
+      <c r="F55" s="134">
+        <v>665.8364527067786</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6871,8 +6920,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="18">
-        <v>15.42567752621673</v>
+      <c r="F56" s="28">
+        <v>48.61807612571168</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6891,8 +6940,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="125">
-        <v>109.559330654955</v>
+      <c r="F57" s="25">
+        <v>210.5029606500208</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6911,8 +6960,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="17">
-        <v>56.80852003835454</v>
+      <c r="F58" s="11">
+        <v>112.6588245471884</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6931,8 +6980,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="18">
-        <v>10.74941146343787</v>
+      <c r="F59" s="9">
+        <v>40.74815128127878</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6951,8 +7000,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="112">
-        <v>85.5994633353298</v>
+      <c r="F60" s="24">
+        <v>162.0789647292588</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6971,8 +7020,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="12">
-        <v>46.5081816047054</v>
+      <c r="F61" s="20">
+        <v>91.66369841781029</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6991,8 +7040,8 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="9">
-        <v>0.1834627105676357</v>
+      <c r="F62" s="130">
+        <v>178.8766223367151</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -7011,8 +7060,8 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="127">
-        <v>198.6769964578388</v>
+      <c r="F63" s="135">
+        <v>651.9960174181306</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -7031,8 +7080,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="112">
-        <v>79.96340726237918</v>
+      <c r="F64" s="136">
+        <v>763.9042786128099</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -7051,8 +7100,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="9">
-        <v>0.1820622210973538</v>
+      <c r="F65" s="126">
+        <v>59.1926191970166</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -7071,8 +7120,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="12">
-        <v>46.27138301571736</v>
+      <c r="F66" s="137">
+        <v>385.2919881290142</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -7091,8 +7140,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="9">
-        <v>2.246918086020362</v>
+      <c r="F67" s="118">
+        <v>345.6120651611868</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -7111,8 +7160,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="9">
-        <v>0.182552994935995</v>
+      <c r="F68" s="26">
+        <v>24.60285722240639</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -7131,8 +7180,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="9">
-        <v>3.172390578078132</v>
+      <c r="F69" s="21">
+        <v>153.5195695893382</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7151,8 +7200,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="9">
-        <v>2.247809531160659</v>
+      <c r="F70" s="27">
+        <v>75.54565155673205</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -7171,8 +7220,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="9">
-        <v>0.1414736227542157</v>
+      <c r="F71" s="26">
+        <v>19.58147479282532</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -7191,8 +7240,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="9">
-        <v>0.4956833922068945</v>
+      <c r="F72" s="10">
+        <v>116.3049573855315</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -7211,8 +7260,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="9">
-        <v>1.973204032884826</v>
+      <c r="F73" s="17">
+        <v>62.35742076885559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>